<commit_message>
updated definitions - Core Java
updated definitions - Core Java
</commit_message>
<xml_diff>
--- a/Definitions.xlsx
+++ b/Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="1807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="1848">
   <si>
     <t>JDK</t>
   </si>
@@ -13434,12 +13434,246 @@
   <si>
     <t>refer u_Stream.collect_method.doc in (JavaPrep\images\1_core_java)</t>
   </si>
+  <si>
+    <t>Parallelism in Collection framewrk</t>
+  </si>
+  <si>
+    <t>Parallel computing involves dividing a problem into subproblems, solving those problems simultaneously (in parallel, with each subproblem running in a separate thread), and then combining the results of the solutions to the subproblems. Java SE provides the fork/join framework, which enables you to more easily implement parallel computing in your applications. However, with this framework, you must specify how the problems are subdivided (partitioned). With aggregate operations, the Java runtime performs this partitioning and combining of solutions for you.</t>
+  </si>
+  <si>
+    <t>One difficulty in implementing parallelism in applications that use collections is that collections are not thread-safe, which means that multiple threads cannot manipulate a collection without introducing thread interference or memory consistency errors. The Collections Framework provides synchronization wrappers, which add automatic synchronization to an arbitrary collection, making it thread-safe. However, synchronization introduces thread contention. You want to avoid thread contention because it prevents threads from running in parallel. Aggregate operations and parallel streams enable you to implement parallelism with non-thread-safe collections provided that you do not modify the collection while you are operating on it.</t>
+  </si>
+  <si>
+    <t>Stream.reduce, Stream.collect</t>
+  </si>
+  <si>
+    <t>parallel grouping based on gender</t>
+  </si>
+  <si>
+    <t>Above is called a concurrent reduction. The Java runtime performs a concurrent reduction if all of the the following are true for a particular pipeline that contains the collect operation:</t>
+  </si>
+  <si>
+    <t>1. The stream is parallel.
+2. The parameter of the collect operation, the collector, has the characteristic Collector.Characteristics.CONCURRENT. To determine the characteristics of a collector, invoke the Collector.characteristics method.
+3. Either the stream is unordered, or the collector has the characteristic Collector.Characteristics.UNORDERED. To ensure that the stream is unordered, invoke the BaseStream.unordered operation.</t>
+  </si>
+  <si>
+    <t>ConcurrentMap&lt;Person.Sex, List&lt;Person&gt;&gt; genderGrouping = persons.parallelStream()
+    .collect(Collectors.groupingByConcurrent(Person::getGender));</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This example returns an instance of ConcurrentMap instead of Map and invokes the groupingByConcurrent operation instead of groupingBy. (See the section Concurrent Collections for more information about ConcurrentMap.) Unlike the operation groupingByConcurrent, the operation groupingBy performs poorly with parallel streams. (This is because it operates by merging two maps by key, which is computationally expensive.) Similarly, the operation Collectors.toConcurrentMap performs better with parallel streams than the operation Collectors.toMap.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ordering collection elements</t>
+  </si>
+  <si>
+    <t>refer v_ordering_collection_elements.doc in (JavaPrep\images\1_core_java)</t>
+  </si>
+  <si>
+    <t>A sequence of aggregate operations is known as a</t>
+  </si>
+  <si>
+    <t>Interview questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pipeline </t>
+  </si>
+  <si>
+    <t>Each pipeline contains zero or more ___ operations</t>
+  </si>
+  <si>
+    <t>Intermediate </t>
+  </si>
+  <si>
+    <t>Each pipeline ends with a ___ operation. </t>
+  </si>
+  <si>
+    <t>Terminal </t>
+  </si>
+  <si>
+    <t>What kind of operation produces another stream as its output? </t>
+  </si>
+  <si>
+    <r>
+      <t>Describe one way in which the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>forEach</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> aggregate operation differs from the enhanced </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> statement or iterators. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The forEach aggregate operation lets the system decide "how" the iteration takes place. Using aggregate operations lets you focus on "what" instead of "how." </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True or False: A stream is similar to a collection in that it is a data structure that stores elements. </t>
+  </si>
+  <si>
+    <t>False. Unlike a collection, a stream is not a data structure. It instead carries values from a source through a pipeline</t>
+  </si>
+  <si>
+    <t>Identify the intermediate and terminal operations in this code:
+double average = roster .stream().filter(p -&gt; p.getGender() == Person.Sex.MALE).mapToInt(Person::getAge).average().getAsDouble();</t>
+  </si>
+  <si>
+    <t>Intermediate: filter, mapToInt, Terminal: average
+The terminal operation average returns an OptionalDouble. The getAsDouble method is then invoked on that returned object.
+It is always a good idea to consult the API Specification for information about whether an operation is intermediate or terminal.</t>
+  </si>
+  <si>
+    <t>The code p -&gt; p.getGender() == Person.Sex.MALE is an example of what?</t>
+  </si>
+  <si>
+    <t>lambda expression</t>
+  </si>
+  <si>
+    <t>The code Person::getAge is an example of what</t>
+  </si>
+  <si>
+    <t>method reference</t>
+  </si>
+  <si>
+    <t>Terminal operations that combine the contents of a stream and return one value are known as what</t>
+  </si>
+  <si>
+    <t>Reduction operations</t>
+  </si>
+  <si>
+    <t>Name one important difference between the Stream.reduce method and the Stream.collect method</t>
+  </si>
+  <si>
+    <t>Stream.reduce always creates a new value when it processes an element. Stream.collect modifies (or mutates) the existing value</t>
+  </si>
+  <si>
+    <t>If you wanted to process a stream of names, extract the male names, and store them in a new List, would Stream.reduce or Stream.collect be the most appropriate operation to use?</t>
+  </si>
+  <si>
+    <t>The collect operation is most appropriate for collecting into a List
+Example:
+List&lt;String&gt; namesOfMaleMembersCollect = roster.stream().filter(p -&gt; p.getGender() == Person.Sex.MALE)
+    .map(p -&gt; p.getName()).collect(Collectors.toList());</t>
+  </si>
+  <si>
+    <t>True or False: Aggregate operations make it possible to implement parallelism with non-thread-safe collections</t>
+  </si>
+  <si>
+    <t>True, provided that you do not modify (mutate) the underlying collection while you are operating on it</t>
+  </si>
+  <si>
+    <t>Streams are always serial unless otherwise specified. How do you request that a stream be processed in parallel?</t>
+  </si>
+  <si>
+    <t>Obtain the parallel stream by invoking parallelStream() instead of stream()</t>
+  </si>
+  <si>
+    <t>List&lt;Album&gt; favs = new ArrayList&lt;&gt;();
+for (Album a : albums) {
+    boolean hasFavorite = false;
+    for (Track t : a.tracks) {
+        if (t.rating &gt;= 4) {
+            hasFavorite = true;
+            break;
+        }
+    }
+    if (hasFavorite)
+        favs.add(a);
+}
+Collections.sort(favs, new Comparator&lt;Album&gt;() {
+                           public int compare(Album a1, Album a2) {
+                               return a1.name.compareTo(a2.name);
+                           }});</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Same functionality with collection stream aggregate functions:
+List&lt;Album&gt; sortedFavs =
+  albums.stream()
+        .filter(a -&gt; a.tracks.anyMatch(t -&gt; (t.rating &gt;= 4)))
+        .sorted(Comparator.comparing(a -&gt; a.name))
+        .collect(Collectors.toList());
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Here we have used the stream operations to simplify each of the three major steps -- identification of whether any track in an album has a rating of at least 4 (anyMatch), the sorting, and the collection of albums matching our criteria into a List. The Comparator.comparing() method takes a function that extracts a Comparable sort key, and returns a Comparator that compares on that key.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13512,6 +13746,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -13594,7 +13840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -13731,20 +13977,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -14056,8 +14311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14239,87 +14494,87 @@
       <c r="C25" s="32"/>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B27" s="27"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>903</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+    <row r="29" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>606</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="C30" s="27"/>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>674</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>1244</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>1333</v>
+        <v>674</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>1244</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>1263</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>1264</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>1262</v>
+        <v>1263</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>1264</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>1262</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B37" s="27"/>
+        <v>283</v>
+      </c>
       <c r="C37" s="41"/>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -14609,9 +14864,9 @@
     <hyperlink ref="B46" r:id="rId8"/>
     <hyperlink ref="B56" r:id="rId9"/>
     <hyperlink ref="B40" r:id="rId10"/>
-    <hyperlink ref="B32" r:id="rId11"/>
+    <hyperlink ref="B33" r:id="rId11"/>
     <hyperlink ref="B17" r:id="rId12"/>
-    <hyperlink ref="B34" r:id="rId13"/>
+    <hyperlink ref="B35" r:id="rId13"/>
     <hyperlink ref="B71" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14621,16 +14876,150 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="102.140625" customWidth="1"/>
+    <col min="1" max="1" width="70.28515625" style="47" customWidth="1"/>
+    <col min="2" max="2" width="113.28515625" style="47" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B1" s="51"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="49" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="47" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A16" s="47" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14650,10 +15039,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>698</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -14715,10 +15104,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B278"/>
+  <dimension ref="A1:B285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
-      <selection activeCell="A279" sqref="A279"/>
+    <sheetView topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="B286" sqref="B286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14728,10 +15117,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -16867,7 +17256,7 @@
       </c>
     </row>
     <row r="269" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A269" s="1" t="s">
+      <c r="A269" s="48" t="s">
         <v>1788</v>
       </c>
       <c r="B269" s="2" t="s">
@@ -16923,32 +17312,86 @@
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="1" t="s">
-        <v>1801</v>
+      <c r="A276" s="47" t="s">
+        <v>125</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>1802</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>1803</v>
+        <v>1801</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
         <v>1805</v>
       </c>
-      <c r="B278" s="2" t="s">
+      <c r="B279" s="2" t="s">
         <v>1806</v>
       </c>
     </row>
+    <row r="280" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A280" s="52" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A281" s="52"/>
+      <c r="B281" s="2" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A283" s="52" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A284" s="52"/>
+      <c r="B284" s="2" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>1817</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A280:A281"/>
+    <mergeCell ref="A283:A284"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -16970,10 +17413,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>902</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -17596,10 +18039,10 @@
       <c r="B79" s="23"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="47" t="s">
+      <c r="A80" s="50" t="s">
         <v>1224</v>
       </c>
-      <c r="B80" s="48"/>
+      <c r="B80" s="51"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -17807,10 +18250,10 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="47" t="s">
+      <c r="A107" s="50" t="s">
         <v>1230</v>
       </c>
-      <c r="B107" s="48"/>
+      <c r="B107" s="51"/>
     </row>
     <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="26" t="s">
@@ -17869,10 +18312,10 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="47" t="s">
+      <c r="A115" s="50" t="s">
         <v>1229</v>
       </c>
-      <c r="B115" s="48"/>
+      <c r="B115" s="51"/>
     </row>
     <row r="116" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
@@ -18155,10 +18598,10 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="47" t="s">
+      <c r="A152" s="50" t="s">
         <v>1195</v>
       </c>
-      <c r="B152" s="48"/>
+      <c r="B152" s="51"/>
     </row>
     <row r="153" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
@@ -18201,10 +18644,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -18503,10 +18946,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="53" t="s">
         <v>435</v>
       </c>
-      <c r="B39" s="49"/>
+      <c r="B39" s="53"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -18701,10 +19144,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="47" t="s">
+      <c r="A65" s="50" t="s">
         <v>500</v>
       </c>
-      <c r="B65" s="48"/>
+      <c r="B65" s="51"/>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
@@ -18867,10 +19310,10 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="47" t="s">
+      <c r="A87" s="50" t="s">
         <v>1246</v>
       </c>
-      <c r="B87" s="48"/>
+      <c r="B87" s="51"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
@@ -18907,10 +19350,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -19393,10 +19836,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -19583,7 +20026,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="54" t="s">
         <v>1070</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -19591,13 +20034,13 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="2" t="s">
         <v>1061</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="54" t="s">
         <v>1071</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -19605,13 +20048,13 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="2" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="52" t="s">
         <v>1072</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -19619,19 +20062,19 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="51"/>
+      <c r="A30" s="52"/>
       <c r="B30" s="3" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="51"/>
+      <c r="A31" s="52"/>
       <c r="B31" s="2" t="s">
         <v>1068</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
+      <c r="A32" s="52"/>
       <c r="B32" s="2" t="s">
         <v>1069</v>
       </c>
@@ -19669,10 +20112,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="s">
+      <c r="A37" s="50" t="s">
         <v>988</v>
       </c>
-      <c r="B37" s="48"/>
+      <c r="B37" s="51"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -19723,10 +20166,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="47" t="s">
+      <c r="A45" s="50" t="s">
         <v>1001</v>
       </c>
-      <c r="B45" s="48"/>
+      <c r="B45" s="51"/>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -19817,7 +20260,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="50" t="s">
+      <c r="A57" s="54" t="s">
         <v>1024</v>
       </c>
       <c r="B57" s="18" t="s">
@@ -19825,7 +20268,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="50"/>
+      <c r="A58" s="54"/>
       <c r="B58" s="18" t="s">
         <v>1026</v>
       </c>
@@ -19847,7 +20290,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="50" t="s">
+      <c r="A61" s="54" t="s">
         <v>1031</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -19855,7 +20298,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="50"/>
+      <c r="A62" s="54"/>
       <c r="B62" s="18" t="s">
         <v>1033</v>
       </c>
@@ -19885,10 +20328,10 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="47" t="s">
+      <c r="A67" s="50" t="s">
         <v>1040</v>
       </c>
-      <c r="B67" s="48"/>
+      <c r="B67" s="51"/>
     </row>
     <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -19986,10 +20429,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>1228</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -20100,10 +20543,10 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="50" t="s">
         <v>1696</v>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="51"/>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -20234,7 +20677,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="54" t="s">
         <v>1768</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -20242,7 +20685,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
+      <c r="A34" s="54"/>
       <c r="B34" s="2" t="s">
         <v>1771</v>
       </c>
@@ -20279,7 +20722,7 @@
   <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20289,10 +20732,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>1473</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
@@ -20791,10 +21234,10 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="47" t="s">
+      <c r="A64" s="50" t="s">
         <v>1474</v>
       </c>
-      <c r="B64" s="48"/>
+      <c r="B64" s="51"/>
     </row>
     <row r="65" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="44" t="s">
@@ -21229,10 +21672,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>607</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -21426,10 +21869,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="50" t="s">
         <v>1265</v>
       </c>
-      <c r="B27" s="48"/>
+      <c r="B27" s="51"/>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -21704,10 +22147,10 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="47" t="s">
+      <c r="A62" s="50" t="s">
         <v>1568</v>
       </c>
-      <c r="B62" s="48"/>
+      <c r="B62" s="51"/>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -21750,7 +22193,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="50" t="s">
+      <c r="A68" s="54" t="s">
         <v>1580</v>
       </c>
       <c r="B68" s="40" t="s">
@@ -21758,7 +22201,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="50"/>
+      <c r="A69" s="54"/>
       <c r="B69" s="40" t="s">
         <v>1582</v>
       </c>

</xml_diff>

<commit_message>
updated collections parallel stream side effects
updated collections parallel stream side effects
</commit_message>
<xml_diff>
--- a/Definitions.xlsx
+++ b/Definitions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="1859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="1869">
   <si>
     <t>JDK</t>
   </si>
@@ -13701,6 +13701,36 @@
   </si>
   <si>
     <t>Clustering</t>
+  </si>
+  <si>
+    <t>JBOSS reference documentation by Redhat</t>
+  </si>
+  <si>
+    <t>https://access.redhat.com/documentation/en-US/index.html</t>
+  </si>
+  <si>
+    <t>min, max, sum, count, average etc</t>
+  </si>
+  <si>
+    <t>Coding Sites</t>
+  </si>
+  <si>
+    <t>https://www.hackerearth.com</t>
+  </si>
+  <si>
+    <t>avinashbabu.donthu@gmail.com/ha0s5t</t>
+  </si>
+  <si>
+    <t>http://www.spoj.com/</t>
+  </si>
+  <si>
+    <t>http://www.topcoder.com/</t>
+  </si>
+  <si>
+    <t>Wildfly</t>
+  </si>
+  <si>
+    <t>https://docs.jboss.org/author/display/WFLY8/Remote+EJB+invocations+via+JNDI+-+EJB+client+API+or+remote-naming+project?_sscc=t</t>
   </si>
 </sst>
 </file>
@@ -13874,7 +13904,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -14018,6 +14048,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -14346,10 +14379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14906,32 +14939,75 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>1715</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>1716</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>1754</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>1756</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>1858</v>
       </c>
     </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="52" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B88" s="53"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
+        <v>1863</v>
+      </c>
+      <c r="B89" s="51" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
+        <v>1866</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A88:B88"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
     <hyperlink ref="B68" r:id="rId2"/>
@@ -14952,9 +15028,11 @@
     <hyperlink ref="B30" r:id="rId17"/>
     <hyperlink ref="B34" r:id="rId18" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
     <hyperlink ref="B33" r:id="rId19"/>
+    <hyperlink ref="B86" r:id="rId20"/>
+    <hyperlink ref="B87" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -14973,10 +15051,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>1818</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
@@ -15123,10 +15201,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>698</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -15190,8 +15268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B286"/>
   <sheetViews>
-    <sheetView topLeftCell="A282" workbookViewId="0">
-      <selection activeCell="A287" sqref="A287"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15201,10 +15279,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -15915,7 +15993,7 @@
         <v>205</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>365</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -17428,7 +17506,7 @@
       </c>
     </row>
     <row r="280" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A280" s="53" t="s">
+      <c r="A280" s="54" t="s">
         <v>1806</v>
       </c>
       <c r="B280" s="2" t="s">
@@ -17436,7 +17514,7 @@
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A281" s="53"/>
+      <c r="A281" s="54"/>
       <c r="B281" s="2" t="s">
         <v>1808</v>
       </c>
@@ -17450,7 +17528,7 @@
       </c>
     </row>
     <row r="283" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A283" s="53" t="s">
+      <c r="A283" s="54" t="s">
         <v>1811</v>
       </c>
       <c r="B283" s="2" t="s">
@@ -17458,7 +17536,7 @@
       </c>
     </row>
     <row r="284" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A284" s="53"/>
+      <c r="A284" s="54"/>
       <c r="B284" s="2" t="s">
         <v>1814</v>
       </c>
@@ -17505,10 +17583,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>901</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -18131,10 +18209,10 @@
       <c r="B79" s="23"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="51" t="s">
+      <c r="A80" s="52" t="s">
         <v>1223</v>
       </c>
-      <c r="B80" s="52"/>
+      <c r="B80" s="53"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -18342,10 +18420,10 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="51" t="s">
+      <c r="A107" s="52" t="s">
         <v>1229</v>
       </c>
-      <c r="B107" s="52"/>
+      <c r="B107" s="53"/>
     </row>
     <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="26" t="s">
@@ -18404,10 +18482,10 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="51" t="s">
+      <c r="A115" s="52" t="s">
         <v>1228</v>
       </c>
-      <c r="B115" s="52"/>
+      <c r="B115" s="53"/>
     </row>
     <row r="116" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
@@ -18690,10 +18768,10 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="51" t="s">
+      <c r="A152" s="52" t="s">
         <v>1194</v>
       </c>
-      <c r="B152" s="52"/>
+      <c r="B152" s="53"/>
     </row>
     <row r="153" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
@@ -18736,10 +18814,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -19038,10 +19116,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="55" t="s">
         <v>435</v>
       </c>
-      <c r="B39" s="54"/>
+      <c r="B39" s="55"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -19236,10 +19314,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="51" t="s">
+      <c r="A65" s="52" t="s">
         <v>500</v>
       </c>
-      <c r="B65" s="52"/>
+      <c r="B65" s="53"/>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
@@ -19402,10 +19480,10 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="51" t="s">
+      <c r="A87" s="52" t="s">
         <v>1245</v>
       </c>
-      <c r="B87" s="52"/>
+      <c r="B87" s="53"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
@@ -19442,10 +19520,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -19928,10 +20006,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -20118,7 +20196,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="56" t="s">
         <v>1069</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -20126,13 +20204,13 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="2" t="s">
         <v>1060</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="56" t="s">
         <v>1070</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -20140,13 +20218,13 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="2" t="s">
         <v>1062</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="54" t="s">
         <v>1071</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -20154,19 +20232,19 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="3" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="2" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="2" t="s">
         <v>1068</v>
       </c>
@@ -20204,10 +20282,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="52" t="s">
         <v>987</v>
       </c>
-      <c r="B37" s="52"/>
+      <c r="B37" s="53"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -20258,10 +20336,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="52" t="s">
         <v>1000</v>
       </c>
-      <c r="B45" s="52"/>
+      <c r="B45" s="53"/>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -20352,7 +20430,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="55" t="s">
+      <c r="A57" s="56" t="s">
         <v>1023</v>
       </c>
       <c r="B57" s="18" t="s">
@@ -20360,7 +20438,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="55"/>
+      <c r="A58" s="56"/>
       <c r="B58" s="18" t="s">
         <v>1025</v>
       </c>
@@ -20382,7 +20460,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="55" t="s">
+      <c r="A61" s="56" t="s">
         <v>1030</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -20390,7 +20468,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="55"/>
+      <c r="A62" s="56"/>
       <c r="B62" s="18" t="s">
         <v>1032</v>
       </c>
@@ -20420,10 +20498,10 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="51" t="s">
+      <c r="A67" s="52" t="s">
         <v>1039</v>
       </c>
-      <c r="B67" s="52"/>
+      <c r="B67" s="53"/>
     </row>
     <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -20521,10 +20599,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>1227</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -20635,10 +20713,10 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="52" t="s">
         <v>1695</v>
       </c>
-      <c r="B16" s="52"/>
+      <c r="B16" s="53"/>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -20769,7 +20847,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="55" t="s">
+      <c r="A33" s="56" t="s">
         <v>1767</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -20777,7 +20855,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="2" t="s">
         <v>1770</v>
       </c>
@@ -20824,10 +20902,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>1472</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
@@ -21326,10 +21404,10 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="51" t="s">
+      <c r="A64" s="52" t="s">
         <v>1473</v>
       </c>
-      <c r="B64" s="52"/>
+      <c r="B64" s="53"/>
     </row>
     <row r="65" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="44" t="s">
@@ -21764,10 +21842,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>607</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -21961,10 +22039,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="52" t="s">
         <v>1264</v>
       </c>
-      <c r="B27" s="52"/>
+      <c r="B27" s="53"/>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -22239,10 +22317,10 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="51" t="s">
+      <c r="A62" s="52" t="s">
         <v>1567</v>
       </c>
-      <c r="B62" s="52"/>
+      <c r="B62" s="53"/>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -22285,7 +22363,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="55" t="s">
+      <c r="A68" s="56" t="s">
         <v>1579</v>
       </c>
       <c r="B68" s="40" t="s">
@@ -22293,7 +22371,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="55"/>
+      <c r="A69" s="56"/>
       <c r="B69" s="40" t="s">
         <v>1581</v>
       </c>

</xml_diff>

<commit_message>
added Linked list questions in algorithms tab
added Linked list questions in algorithms tab
</commit_message>
<xml_diff>
--- a/Definitions.xlsx
+++ b/Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="3" r:id="rId1"/>
@@ -17,14 +17,14 @@
     <sheet name="Servlets-JSP" sheetId="10" r:id="rId8"/>
     <sheet name="Tools" sheetId="8" r:id="rId9"/>
     <sheet name="Java Interview Ques" sheetId="11" r:id="rId10"/>
-    <sheet name="Amazon interview prep" sheetId="4" r:id="rId11"/>
+    <sheet name="Algorithms" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="1869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="1887">
   <si>
     <t>JDK</t>
   </si>
@@ -13731,6 +13731,60 @@
   </si>
   <si>
     <t>https://docs.jboss.org/author/display/WFLY8/Remote+EJB+invocations+via+JNDI+-+EJB+client+API+or+remote-naming+project?_sscc=t</t>
+  </si>
+  <si>
+    <t>Linked List questions</t>
+  </si>
+  <si>
+    <t>how will you find the middle of the linked list - 2 pointer approach</t>
+  </si>
+  <si>
+    <t>how will you display the linked list from end - stack</t>
+  </si>
+  <si>
+    <t>check whether given linked list is even or odd</t>
+  </si>
+  <si>
+    <t>if head of the linked list is pointing to kth element, how will you get the elements before kth  element</t>
+  </si>
+  <si>
+    <t>given two sorted linked lists, we need to merge them into third linked list in sorted order</t>
+  </si>
+  <si>
+    <t>reverse the linked list in pairs, input: 1-&gt;2-&gt;3-&gt;4-&gt;X, output:2-&gt;1-&gt;4-&gt;3-&gt;X</t>
+  </si>
+  <si>
+    <t>given a binary tree, convert it into doubly linked list</t>
+  </si>
+  <si>
+    <t>sort the linked list</t>
+  </si>
+  <si>
+    <t>split the circular linked list into two equal parts. if the number of nodes in the list are odd then make a first list one node extra than second list</t>
+  </si>
+  <si>
+    <t>how will you check if linked list is palindrome or not?</t>
+  </si>
+  <si>
+    <t>exchange adjucent elements in a linked list</t>
+  </si>
+  <si>
+    <t>for a give value K (K&gt;0) reverse block of K nodes in a list. Input: 1,2,3,4,5,6,7,8,9 output: 2: 2,1,4,3,6,5,8,7,9; output:3:3,2,1,6,5,4,9,8,7</t>
+  </si>
+  <si>
+    <t>JosephusCircle</t>
+  </si>
+  <si>
+    <t>given a linked list consists of data, next pointer and also a random pointer which points to a random node of a list. Give an algorithm for the cloning the list</t>
+  </si>
+  <si>
+    <t>Find a cycle in linked list</t>
+  </si>
+  <si>
+    <t>find the length of linked list</t>
+  </si>
+  <si>
+    <t>find kth element from last in a linked list</t>
   </si>
 </sst>
 </file>
@@ -13904,7 +13958,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -14048,6 +14102,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -14381,7 +14438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
@@ -14981,10 +15038,10 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="52" t="s">
+      <c r="A88" s="53" t="s">
         <v>1862</v>
       </c>
-      <c r="B88" s="53"/>
+      <c r="B88" s="54"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
@@ -15040,8 +15097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15051,10 +15108,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>1818</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
@@ -15187,73 +15244,165 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="1" max="1" width="123.7109375" style="52" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
     <col min="5" max="5" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>698</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="52" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>360</v>
-      </c>
-    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>362</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="53" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B11" s="54"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="52" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52" t="s">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="52" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
+        <v>1886</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1" display="http://www.geeksforgeeks.org/amazon-interview-set-27/"/>
@@ -15279,10 +15428,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -17441,7 +17590,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="45" t="s">
         <v>1793</v>
       </c>
@@ -17506,7 +17655,7 @@
       </c>
     </row>
     <row r="280" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A280" s="54" t="s">
+      <c r="A280" s="55" t="s">
         <v>1806</v>
       </c>
       <c r="B280" s="2" t="s">
@@ -17514,7 +17663,7 @@
       </c>
     </row>
     <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A281" s="54"/>
+      <c r="A281" s="55"/>
       <c r="B281" s="2" t="s">
         <v>1808</v>
       </c>
@@ -17528,7 +17677,7 @@
       </c>
     </row>
     <row r="283" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A283" s="54" t="s">
+      <c r="A283" s="55" t="s">
         <v>1811</v>
       </c>
       <c r="B283" s="2" t="s">
@@ -17536,7 +17685,7 @@
       </c>
     </row>
     <row r="284" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A284" s="54"/>
+      <c r="A284" s="55"/>
       <c r="B284" s="2" t="s">
         <v>1814</v>
       </c>
@@ -17583,10 +17732,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>901</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -18209,10 +18358,10 @@
       <c r="B79" s="23"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="52" t="s">
+      <c r="A80" s="53" t="s">
         <v>1223</v>
       </c>
-      <c r="B80" s="53"/>
+      <c r="B80" s="54"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -18420,10 +18569,10 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="52" t="s">
+      <c r="A107" s="53" t="s">
         <v>1229</v>
       </c>
-      <c r="B107" s="53"/>
+      <c r="B107" s="54"/>
     </row>
     <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="26" t="s">
@@ -18482,10 +18631,10 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="52" t="s">
+      <c r="A115" s="53" t="s">
         <v>1228</v>
       </c>
-      <c r="B115" s="53"/>
+      <c r="B115" s="54"/>
     </row>
     <row r="116" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
@@ -18768,10 +18917,10 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="52" t="s">
+      <c r="A152" s="53" t="s">
         <v>1194</v>
       </c>
-      <c r="B152" s="53"/>
+      <c r="B152" s="54"/>
     </row>
     <row r="153" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
@@ -18814,10 +18963,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -19116,10 +19265,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="56" t="s">
         <v>435</v>
       </c>
-      <c r="B39" s="55"/>
+      <c r="B39" s="56"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -19314,10 +19463,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="52" t="s">
+      <c r="A65" s="53" t="s">
         <v>500</v>
       </c>
-      <c r="B65" s="53"/>
+      <c r="B65" s="54"/>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
@@ -19480,10 +19629,10 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="52" t="s">
+      <c r="A87" s="53" t="s">
         <v>1245</v>
       </c>
-      <c r="B87" s="53"/>
+      <c r="B87" s="54"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
@@ -19520,10 +19669,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -20006,10 +20155,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -20196,7 +20345,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="57" t="s">
         <v>1069</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -20204,13 +20353,13 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
+      <c r="A26" s="57"/>
       <c r="B26" s="2" t="s">
         <v>1060</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="57" t="s">
         <v>1070</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -20218,13 +20367,13 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="2" t="s">
         <v>1062</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="55" t="s">
         <v>1071</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -20232,19 +20381,19 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
+      <c r="A30" s="55"/>
       <c r="B30" s="3" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
+      <c r="A31" s="55"/>
       <c r="B31" s="2" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
+      <c r="A32" s="55"/>
       <c r="B32" s="2" t="s">
         <v>1068</v>
       </c>
@@ -20282,10 +20431,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="52" t="s">
+      <c r="A37" s="53" t="s">
         <v>987</v>
       </c>
-      <c r="B37" s="53"/>
+      <c r="B37" s="54"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -20336,10 +20485,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="52" t="s">
+      <c r="A45" s="53" t="s">
         <v>1000</v>
       </c>
-      <c r="B45" s="53"/>
+      <c r="B45" s="54"/>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -20430,7 +20579,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="57" t="s">
         <v>1023</v>
       </c>
       <c r="B57" s="18" t="s">
@@ -20438,7 +20587,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="56"/>
+      <c r="A58" s="57"/>
       <c r="B58" s="18" t="s">
         <v>1025</v>
       </c>
@@ -20460,7 +20609,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="56" t="s">
+      <c r="A61" s="57" t="s">
         <v>1030</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -20468,7 +20617,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="56"/>
+      <c r="A62" s="57"/>
       <c r="B62" s="18" t="s">
         <v>1032</v>
       </c>
@@ -20498,10 +20647,10 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="52" t="s">
+      <c r="A67" s="53" t="s">
         <v>1039</v>
       </c>
-      <c r="B67" s="53"/>
+      <c r="B67" s="54"/>
     </row>
     <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -20599,10 +20748,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>1227</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -20713,10 +20862,10 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="53" t="s">
         <v>1695</v>
       </c>
-      <c r="B16" s="53"/>
+      <c r="B16" s="54"/>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -20847,7 +20996,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="57" t="s">
         <v>1767</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -20855,7 +21004,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
+      <c r="A34" s="57"/>
       <c r="B34" s="2" t="s">
         <v>1770</v>
       </c>
@@ -20902,10 +21051,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>1472</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
@@ -21404,10 +21553,10 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="52" t="s">
+      <c r="A64" s="53" t="s">
         <v>1473</v>
       </c>
-      <c r="B64" s="53"/>
+      <c r="B64" s="54"/>
     </row>
     <row r="65" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="44" t="s">
@@ -21842,10 +21991,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>607</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -22039,10 +22188,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="53" t="s">
         <v>1264</v>
       </c>
-      <c r="B27" s="53"/>
+      <c r="B27" s="54"/>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -22317,10 +22466,10 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="52" t="s">
+      <c r="A62" s="53" t="s">
         <v>1567</v>
       </c>
-      <c r="B62" s="53"/>
+      <c r="B62" s="54"/>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -22363,7 +22512,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="56" t="s">
+      <c r="A68" s="57" t="s">
         <v>1579</v>
       </c>
       <c r="B68" s="40" t="s">
@@ -22371,7 +22520,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="56"/>
+      <c r="A69" s="57"/>
       <c r="B69" s="40" t="s">
         <v>1581</v>
       </c>

</xml_diff>

<commit_message>
Core java definitions updated
Core java definitions updated
</commit_message>
<xml_diff>
--- a/Definitions.xlsx
+++ b/Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="1887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="1893">
   <si>
     <t>JDK</t>
   </si>
@@ -12376,9 +12376,6 @@
   </si>
   <si>
     <t>GitHub</t>
-  </si>
-  <si>
-    <t>@SuppressWarnings("deprecation","unchecked","rawtypes", "serial", "unused");</t>
   </si>
   <si>
     <t>REST Web Services</t>
@@ -13785,6 +13782,27 @@
   </si>
   <si>
     <t>find kth element from last in a linked list</t>
+  </si>
+  <si>
+    <t>@SuppressWarnings("deprecation","unchecked","rawtypes", "serial", "unused","null");</t>
+  </si>
+  <si>
+    <t>Memory efficient linked list. XOR linked list</t>
+  </si>
+  <si>
+    <t>Stack functionalities - push, pop, top, size, isEmpty, isFull</t>
+  </si>
+  <si>
+    <t>Stack implementations - simple array, dynamic array(uses array doubling), linked list</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Discuss how stack can be used for checking balancing of symbols</t>
+  </si>
+  <si>
+    <t>Discuss Infix to postfix conversion algorithm using stack</t>
   </si>
 </sst>
 </file>
@@ -13958,7 +13976,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -14111,6 +14129,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14541,7 +14562,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -14643,16 +14664,16 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>1850</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>1851</v>
       </c>
       <c r="C30" s="50"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="B31" s="50"/>
       <c r="C31" s="50"/>
@@ -14665,19 +14686,19 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>1854</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>1855</v>
       </c>
       <c r="C33" s="50"/>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>1852</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>1853</v>
       </c>
       <c r="C34" s="50"/>
     </row>
@@ -14827,7 +14848,7 @@
         <v>284</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -14917,7 +14938,7 @@
         <v>883</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -14975,90 +14996,90 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>1717</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>1718</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B86" s="6" t="s">
         <v>1859</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>1860</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>1867</v>
       </c>
-      <c r="B87" s="4" t="s">
-        <v>1868</v>
-      </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="53" t="s">
-        <v>1862</v>
-      </c>
-      <c r="B88" s="54"/>
+      <c r="A88" s="54" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B88" s="55"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B89" s="51" t="s">
         <v>1863</v>
-      </c>
-      <c r="B89" s="51" t="s">
-        <v>1864</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
     </row>
   </sheetData>
@@ -15108,129 +15129,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>1818</v>
-      </c>
-      <c r="B1" s="54"/>
+      <c r="A1" s="54" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>1820</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>1821</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>1822</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>1823</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>1825</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>1826</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B7" s="47" t="s">
         <v>1827</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>1828</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B8" s="47" t="s">
         <v>1829</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>1830</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B9" s="47" t="s">
         <v>1831</v>
-      </c>
-      <c r="B9" s="47" t="s">
-        <v>1832</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B10" s="47" t="s">
         <v>1833</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>1834</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B11" s="47" t="s">
         <v>1835</v>
-      </c>
-      <c r="B11" s="47" t="s">
-        <v>1836</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B12" s="47" t="s">
         <v>1837</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>1838</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B13" s="47" t="s">
         <v>1839</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>1840</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B14" s="47" t="s">
         <v>1841</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>1842</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B15" s="47" t="s">
         <v>1843</v>
-      </c>
-      <c r="B15" s="47" t="s">
-        <v>1844</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B16" s="48" t="s">
         <v>1845</v>
-      </c>
-      <c r="B16" s="48" t="s">
-        <v>1846</v>
       </c>
     </row>
   </sheetData>
@@ -15244,24 +15265,24 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="123.7109375" style="52" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" style="52" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" style="53" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>698</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
@@ -15309,100 +15330,130 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
-        <v>1869</v>
-      </c>
-      <c r="B11" s="54"/>
+      <c r="A11" s="54" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B11" s="55"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>1873</v>
+        <v>1872</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>1887</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
         <v>1874</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
         <v>1875</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
         <v>1876</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
         <v>1877</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="52" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
         <v>1878</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
         <v>1879</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52" t="s">
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="52" t="s">
         <v>1880</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="52" t="s">
         <v>1881</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52" t="s">
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="52" t="s">
         <v>1882</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="52" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
         <v>1883</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
         <v>1884</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
         <v>1885</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
-        <v>1886</v>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="54" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B29" s="55"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="52" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="52" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="52" t="s">
+        <v>1892</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1" display="http://www.geeksforgeeks.org/amazon-interview-set-27/"/>
@@ -15415,10 +15466,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B286"/>
+  <dimension ref="A1:B288"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15428,10 +15479,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -16142,7 +16193,7 @@
         <v>205</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16422,7 +16473,7 @@
         <v>715</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>1694</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -17520,95 +17571,95 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B263" s="2" t="s">
         <v>1775</v>
-      </c>
-      <c r="B263" s="2" t="s">
-        <v>1776</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B264" s="2" t="s">
         <v>1777</v>
-      </c>
-      <c r="B264" s="2" t="s">
-        <v>1778</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B265" s="2" t="s">
         <v>1779</v>
-      </c>
-      <c r="B265" s="2" t="s">
-        <v>1780</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B266" s="2" t="s">
         <v>1781</v>
-      </c>
-      <c r="B266" s="2" t="s">
-        <v>1782</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B267" s="2" t="s">
         <v>1783</v>
-      </c>
-      <c r="B267" s="2" t="s">
-        <v>1784</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B268" s="2" t="s">
         <v>1785</v>
-      </c>
-      <c r="B268" s="2" t="s">
-        <v>1786</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A269" s="48" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B269" s="2" t="s">
         <v>1787</v>
-      </c>
-      <c r="B269" s="2" t="s">
-        <v>1788</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B270" s="2" t="s">
         <v>1789</v>
-      </c>
-      <c r="B270" s="2" t="s">
-        <v>1790</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B271" s="2" t="s">
         <v>1791</v>
-      </c>
-      <c r="B271" s="2" t="s">
-        <v>1792</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="45" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B272" s="2" t="s">
         <v>1793</v>
-      </c>
-      <c r="B272" s="2" t="s">
-        <v>1794</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B273" s="2" t="s">
         <v>1795</v>
-      </c>
-      <c r="B273" s="2" t="s">
-        <v>1796</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>365</v>
@@ -17616,10 +17667,10 @@
     </row>
     <row r="275" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B275" s="2" t="s">
         <v>1798</v>
-      </c>
-      <c r="B275" s="2" t="s">
-        <v>1799</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
@@ -17627,90 +17678,97 @@
         <v>125</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B277" s="2" t="s">
         <v>1800</v>
-      </c>
-      <c r="B277" s="2" t="s">
-        <v>1801</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B278" s="2" t="s">
         <v>1802</v>
-      </c>
-      <c r="B278" s="2" t="s">
-        <v>1803</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B279" s="2" t="s">
         <v>1804</v>
       </c>
-      <c r="B279" s="2" t="s">
+    </row>
+    <row r="280" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A280" s="56" t="s">
         <v>1805</v>
       </c>
-    </row>
-    <row r="280" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A280" s="55" t="s">
+      <c r="B280" s="2" t="s">
         <v>1806</v>
       </c>
-      <c r="B280" s="2" t="s">
+    </row>
+    <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A281" s="56"/>
+      <c r="B281" s="2" t="s">
         <v>1807</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A281" s="55"/>
-      <c r="B281" s="2" t="s">
-        <v>1808</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A283" s="56" t="s">
         <v>1810</v>
       </c>
-      <c r="B282" s="2" t="s">
+      <c r="B283" s="2" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A284" s="56"/>
+      <c r="B284" s="2" t="s">
         <v>1813</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A283" s="55" t="s">
-        <v>1811</v>
-      </c>
-      <c r="B283" s="2" t="s">
-        <v>1812</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A284" s="55"/>
-      <c r="B284" s="2" t="s">
-        <v>1814</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B285" s="2" t="s">
         <v>1815</v>
-      </c>
-      <c r="B285" s="2" t="s">
-        <v>1816</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>1856</v>
-      </c>
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B288" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A280:A281"/>
     <mergeCell ref="A283:A284"/>
+    <mergeCell ref="A288:B288"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -17732,10 +17790,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>901</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -18358,10 +18416,10 @@
       <c r="B79" s="23"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="53" t="s">
+      <c r="A80" s="54" t="s">
         <v>1223</v>
       </c>
-      <c r="B80" s="54"/>
+      <c r="B80" s="55"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -18569,10 +18627,10 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="53" t="s">
+      <c r="A107" s="54" t="s">
         <v>1229</v>
       </c>
-      <c r="B107" s="54"/>
+      <c r="B107" s="55"/>
     </row>
     <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="26" t="s">
@@ -18631,10 +18689,10 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="53" t="s">
+      <c r="A115" s="54" t="s">
         <v>1228</v>
       </c>
-      <c r="B115" s="54"/>
+      <c r="B115" s="55"/>
     </row>
     <row r="116" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
@@ -18917,10 +18975,10 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="53" t="s">
+      <c r="A152" s="54" t="s">
         <v>1194</v>
       </c>
-      <c r="B152" s="54"/>
+      <c r="B152" s="55"/>
     </row>
     <row r="153" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
@@ -18963,10 +19021,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -19265,10 +19323,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="57" t="s">
         <v>435</v>
       </c>
-      <c r="B39" s="56"/>
+      <c r="B39" s="57"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -19463,10 +19521,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="53" t="s">
+      <c r="A65" s="54" t="s">
         <v>500</v>
       </c>
-      <c r="B65" s="54"/>
+      <c r="B65" s="55"/>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
@@ -19629,10 +19687,10 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="53" t="s">
+      <c r="A87" s="54" t="s">
         <v>1245</v>
       </c>
-      <c r="B87" s="54"/>
+      <c r="B87" s="55"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
@@ -19669,10 +19727,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -20155,10 +20213,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -20345,7 +20403,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="58" t="s">
         <v>1069</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -20353,13 +20411,13 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="57"/>
+      <c r="A26" s="58"/>
       <c r="B26" s="2" t="s">
         <v>1060</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="58" t="s">
         <v>1070</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -20367,13 +20425,13 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="57"/>
+      <c r="A28" s="58"/>
       <c r="B28" s="2" t="s">
         <v>1062</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="56" t="s">
         <v>1071</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -20381,19 +20439,19 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="3" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="2" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="2" t="s">
         <v>1068</v>
       </c>
@@ -20431,10 +20489,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="54" t="s">
         <v>987</v>
       </c>
-      <c r="B37" s="54"/>
+      <c r="B37" s="55"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -20485,10 +20543,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="53" t="s">
+      <c r="A45" s="54" t="s">
         <v>1000</v>
       </c>
-      <c r="B45" s="54"/>
+      <c r="B45" s="55"/>
     </row>
     <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -20579,7 +20637,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="57" t="s">
+      <c r="A57" s="58" t="s">
         <v>1023</v>
       </c>
       <c r="B57" s="18" t="s">
@@ -20587,7 +20645,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="57"/>
+      <c r="A58" s="58"/>
       <c r="B58" s="18" t="s">
         <v>1025</v>
       </c>
@@ -20609,7 +20667,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="57" t="s">
+      <c r="A61" s="58" t="s">
         <v>1030</v>
       </c>
       <c r="B61" s="18" t="s">
@@ -20617,7 +20675,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
+      <c r="A62" s="58"/>
       <c r="B62" s="18" t="s">
         <v>1032</v>
       </c>
@@ -20647,10 +20705,10 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="53" t="s">
+      <c r="A67" s="54" t="s">
         <v>1039</v>
       </c>
-      <c r="B67" s="54"/>
+      <c r="B67" s="55"/>
     </row>
     <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -20748,17 +20806,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>1227</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B2" t="s">
         <v>1698</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1699</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -20855,88 +20913,88 @@
     </row>
     <row r="15" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B15" s="42" t="s">
         <v>1706</v>
       </c>
-      <c r="B15" s="42" t="s">
-        <v>1707</v>
-      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B16" s="54"/>
+      <c r="A16" s="54" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B16" s="55"/>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B17" s="42" t="s">
         <v>1696</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>1697</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B18" t="s">
         <v>1698</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1699</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B19" s="42" t="s">
         <v>1701</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>1702</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B21" s="42" t="s">
         <v>1704</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>1705</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B22" s="42" t="s">
         <v>1708</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>1709</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B24" s="42" t="s">
         <v>1711</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>1712</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B25" s="43" t="s">
         <v>1752</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>1753</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -20949,26 +21007,26 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>1757</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>1758</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>1759</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>1760</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>1761</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>1762</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -20976,53 +21034,53 @@
         <v>1356</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="43" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B32" s="43" t="s">
         <v>1765</v>
       </c>
-      <c r="B32" s="43" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="58" t="s">
         <v>1766</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="57" t="s">
-        <v>1767</v>
-      </c>
       <c r="B33" s="2" t="s">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="58"/>
+      <c r="B34" s="2" t="s">
         <v>1769</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="57"/>
-      <c r="B34" s="2" t="s">
-        <v>1770</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B35" s="43" t="s">
         <v>1771</v>
-      </c>
-      <c r="B35" s="43" t="s">
-        <v>1772</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>1773</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>1774</v>
       </c>
     </row>
   </sheetData>
@@ -21051,10 +21109,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>1472</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
@@ -21077,7 +21135,7 @@
         <v>1360</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -21093,7 +21151,7 @@
         <v>1363</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -21109,7 +21167,7 @@
         <v>1366</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -21149,7 +21207,7 @@
         <v>1386</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -21213,7 +21271,7 @@
         <v>1400</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -21221,7 +21279,7 @@
         <v>1401</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21229,7 +21287,7 @@
         <v>1402</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -21245,7 +21303,7 @@
         <v>1405</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -21277,7 +21335,7 @@
         <v>1386</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -21290,10 +21348,10 @@
     </row>
     <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>1728</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>1729</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -21301,7 +21359,7 @@
         <v>1427</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -21325,7 +21383,7 @@
         <v>1419</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21333,7 +21391,7 @@
         <v>1421</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -21341,7 +21399,7 @@
         <v>1422</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21349,7 +21407,7 @@
         <v>1420</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -21378,10 +21436,10 @@
     </row>
     <row r="42" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="38" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -21397,7 +21455,7 @@
         <v>1434</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -21445,7 +21503,7 @@
         <v>1445</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -21533,7 +21591,7 @@
         <v>1466</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21541,7 +21599,7 @@
         <v>1467</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21549,18 +21607,18 @@
         <v>1468</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="53" t="s">
+      <c r="A64" s="54" t="s">
         <v>1473</v>
       </c>
-      <c r="B64" s="54"/>
+      <c r="B64" s="55"/>
     </row>
     <row r="65" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="44" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="B65" s="43" t="s">
         <v>1520</v>
@@ -21619,7 +21677,7 @@
         <v>1488</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21667,7 +21725,7 @@
         <v>1499</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -21680,7 +21738,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="38" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>1506</v>
@@ -21691,7 +21749,7 @@
         <v>1507</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -21843,12 +21901,12 @@
         <v>1539</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="44" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>1540</v>
@@ -21907,7 +21965,7 @@
         <v>1553</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -21991,10 +22049,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>607</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -22188,10 +22246,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="54" t="s">
         <v>1264</v>
       </c>
-      <c r="B27" s="54"/>
+      <c r="B27" s="55"/>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -22466,10 +22524,10 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="53" t="s">
+      <c r="A62" s="54" t="s">
         <v>1567</v>
       </c>
-      <c r="B62" s="54"/>
+      <c r="B62" s="55"/>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -22512,7 +22570,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="57" t="s">
+      <c r="A68" s="58" t="s">
         <v>1579</v>
       </c>
       <c r="B68" s="40" t="s">
@@ -22520,7 +22578,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="57"/>
+      <c r="A69" s="58"/>
       <c r="B69" s="40" t="s">
         <v>1581</v>
       </c>

</xml_diff>

<commit_message>
core java - jvm
core java - jvm
</commit_message>
<xml_diff>
--- a/Definitions.xlsx
+++ b/Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="1992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="1994">
   <si>
     <t>JDK</t>
   </si>
@@ -14371,6 +14371,16 @@
   </si>
   <si>
     <t>It is possible to define a method that will be called just before an object's final destruction by the garbage collector. This method is called finalize( ), and it can be used to ensure that an object terminates cleanly</t>
+  </si>
+  <si>
+    <t>class having private constructor with sub class - we can not have sub class</t>
+  </si>
+  <si>
+    <t>public class SuperClass1 {
+ private SuperClass1() { }  }
+/*we can not extend class having private constructor
+ * if we remove comments around extends compiler error will come*/
+public class SubClass1 /*extends SuperClass1*/{ }</t>
   </si>
 </sst>
 </file>
@@ -14552,7 +14562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -14739,6 +14749,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -15682,10 +15695,10 @@
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="65" t="s">
+      <c r="A90" s="66" t="s">
         <v>1829</v>
       </c>
-      <c r="B90" s="66"/>
+      <c r="B90" s="67"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
@@ -15741,7 +15754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -15752,10 +15765,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>1785</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
@@ -15918,10 +15931,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>695</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
@@ -15969,10 +15982,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="66" t="s">
         <v>1836</v>
       </c>
-      <c r="B11" s="66"/>
+      <c r="B11" s="67"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
@@ -16063,10 +16076,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="66" t="s">
         <v>1857</v>
       </c>
-      <c r="B29" s="66"/>
+      <c r="B29" s="67"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
@@ -16110,10 +16123,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B353"/>
+  <dimension ref="A1:B356"/>
   <sheetViews>
-    <sheetView topLeftCell="A287" workbookViewId="0">
-      <selection activeCell="B290" sqref="B290"/>
+    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
+      <selection activeCell="A309" sqref="A309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16123,10 +16136,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -16985,7 +16998,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A109" s="67" t="s">
+      <c r="A109" s="68" t="s">
         <v>1774</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -16993,7 +17006,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="67"/>
+      <c r="A110" s="68"/>
       <c r="B110" s="2" t="s">
         <v>1776</v>
       </c>
@@ -17007,7 +17020,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A112" s="67" t="s">
+      <c r="A112" s="68" t="s">
         <v>1778</v>
       </c>
       <c r="B112" s="2" t="s">
@@ -17015,7 +17028,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A113" s="67"/>
+      <c r="A113" s="68"/>
       <c r="B113" s="2" t="s">
         <v>1781</v>
       </c>
@@ -18425,304 +18438,306 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="64"/>
+    <row r="290" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A290" s="65" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>1993</v>
+      </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="65" t="s">
+      <c r="A291" s="64"/>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" s="65"/>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="65"/>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B291" s="66"/>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="53" t="s">
+      <c r="B294" s="67"/>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" s="53" t="s">
         <v>1876</v>
       </c>
-      <c r="B292" s="53" t="s">
+      <c r="B295" s="53" t="s">
         <v>1877</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="53" t="s">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" s="53" t="s">
         <v>1878</v>
       </c>
-      <c r="B293" s="53" t="s">
+      <c r="B296" s="53" t="s">
         <v>1879</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A294" s="53" t="s">
+    <row r="297" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A297" s="53" t="s">
         <v>1935</v>
       </c>
-      <c r="B294" s="53" t="s">
+      <c r="B297" s="53" t="s">
         <v>1883</v>
       </c>
     </row>
-    <row r="295" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A295" s="67" t="s">
+    <row r="298" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A298" s="68" t="s">
         <v>1888</v>
       </c>
-      <c r="B295" s="53" t="s">
+      <c r="B298" s="53" t="s">
         <v>1880</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A296" s="67"/>
-      <c r="B296" s="53" t="s">
+    <row r="299" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A299" s="68"/>
+      <c r="B299" s="53" t="s">
         <v>1881</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A297" s="67"/>
-      <c r="B297" s="53" t="s">
+    <row r="300" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A300" s="68"/>
+      <c r="B300" s="53" t="s">
         <v>1882</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A298" s="53" t="s">
+    <row r="301" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A301" s="53" t="s">
         <v>1884</v>
       </c>
-      <c r="B298" s="53" t="s">
+      <c r="B301" s="53" t="s">
         <v>1885</v>
       </c>
     </row>
-    <row r="299" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A299" s="67" t="s">
+    <row r="302" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A302" s="68" t="s">
         <v>1886</v>
       </c>
-      <c r="B299" s="53" t="s">
+      <c r="B302" s="53" t="s">
         <v>1887</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A300" s="67"/>
-      <c r="B300" s="53" t="s">
+    <row r="303" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A303" s="68"/>
+      <c r="B303" s="53" t="s">
         <v>1936</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="53" t="s">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" s="53" t="s">
         <v>1889</v>
       </c>
-      <c r="B301" s="53" t="s">
+      <c r="B304" s="53" t="s">
         <v>1890</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A302" s="57" t="s">
+    <row r="305" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A305" s="57" t="s">
         <v>1891</v>
       </c>
-      <c r="B302" s="53" t="s">
+      <c r="B305" s="53" t="s">
         <v>1892</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A303" s="57" t="s">
+    <row r="306" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A306" s="57" t="s">
         <v>1893</v>
       </c>
-      <c r="B303" s="53" t="s">
+      <c r="B306" s="53" t="s">
         <v>1937</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A304" s="57" t="s">
+    <row r="307" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A307" s="57" t="s">
         <v>1894</v>
       </c>
-      <c r="B304" s="53" t="s">
+      <c r="B307" s="53" t="s">
         <v>1895</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A305" s="58" t="s">
+    <row r="308" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A308" s="58" t="s">
         <v>1896</v>
       </c>
-      <c r="B305" s="53" t="s">
+      <c r="B308" s="53" t="s">
         <v>1938</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A306" s="57" t="s">
+    <row r="309" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A309" s="57" t="s">
         <v>1897</v>
       </c>
-      <c r="B306" s="53" t="s">
+      <c r="B309" s="53" t="s">
         <v>1898</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="53" t="s">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" s="53" t="s">
         <v>1899</v>
       </c>
-      <c r="B307" s="53" t="s">
+      <c r="B310" s="53" t="s">
         <v>1900</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A308" s="53" t="s">
+    <row r="311" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A311" s="53" t="s">
         <v>1901</v>
       </c>
-      <c r="B308" s="53" t="s">
+      <c r="B311" s="53" t="s">
         <v>1902</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="53" t="s">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" s="53" t="s">
         <v>1903</v>
       </c>
-      <c r="B309" s="53" t="s">
+      <c r="B312" s="53" t="s">
         <v>1904</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A310" s="57" t="s">
-        <v>1905</v>
-      </c>
-      <c r="B310" s="53" t="s">
-        <v>1906</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A311" s="57" t="s">
-        <v>1907</v>
-      </c>
-      <c r="B311" s="53" t="s">
-        <v>1908</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A312" s="57" t="s">
-        <v>1911</v>
-      </c>
-      <c r="B312" s="55" t="s">
-        <v>1912</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A313" s="57" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B313" s="53" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A314" s="57" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B314" s="53" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A315" s="57" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B315" s="55" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A316" s="57" t="s">
         <v>1909</v>
       </c>
-      <c r="B313" s="55" t="s">
+      <c r="B316" s="55" t="s">
         <v>1910</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A314" s="67" t="s">
+    <row r="317" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A317" s="68" t="s">
         <v>1913</v>
       </c>
-      <c r="B314" s="55" t="s">
+      <c r="B317" s="55" t="s">
         <v>1914</v>
       </c>
     </row>
-    <row r="315" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A315" s="67"/>
-      <c r="B315" s="55" t="s">
+    <row r="318" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A318" s="68"/>
+      <c r="B318" s="55" t="s">
         <v>1915</v>
       </c>
     </row>
-    <row r="316" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A316" s="67"/>
-      <c r="B316" s="55" t="s">
+    <row r="319" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A319" s="68"/>
+      <c r="B319" s="55" t="s">
         <v>1916</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="55" t="s">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" s="55" t="s">
         <v>1917</v>
       </c>
-      <c r="B317" s="55" t="s">
+      <c r="B320" s="55" t="s">
         <v>1918</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="55" t="s">
-        <v>1960</v>
-      </c>
-      <c r="B318" s="55" t="s">
-        <v>1961</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="55" t="s">
-        <v>1962</v>
-      </c>
-      <c r="B319" s="55" t="s">
-        <v>1963</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A320" s="55" t="s">
-        <v>1964</v>
-      </c>
-      <c r="B320" s="55" t="s">
-        <v>1965</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="55" t="s">
-        <v>1966</v>
+        <v>1960</v>
       </c>
       <c r="B321" s="55" t="s">
-        <v>1967</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="55" t="s">
-        <v>1968</v>
+        <v>1962</v>
       </c>
       <c r="B322" s="55" t="s">
-        <v>1969</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A323" s="55" t="s">
-        <v>1970</v>
+        <v>1964</v>
       </c>
       <c r="B323" s="55" t="s">
-        <v>1971</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="55" t="s">
-        <v>1972</v>
+        <v>1966</v>
       </c>
       <c r="B324" s="55" t="s">
-        <v>1973</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="55" t="s">
-        <v>1974</v>
+        <v>1968</v>
       </c>
       <c r="B325" s="55" t="s">
-        <v>1975</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="55" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B326" s="55" t="s">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="55" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B327" s="55" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" s="55" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B328" s="55" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="55" t="s">
         <v>1976</v>
       </c>
-      <c r="B326" s="55" t="s">
+      <c r="B329" s="55" t="s">
         <v>1977</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="53" t="s">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" s="53" t="s">
         <v>1978</v>
       </c>
-      <c r="B327" s="53" t="s">
+      <c r="B330" s="53" t="s">
         <v>1979</v>
       </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="62"/>
-      <c r="B328" s="62"/>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="62"/>
-      <c r="B329" s="62"/>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="62"/>
-      <c r="B330" s="62"/>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="62"/>
@@ -18784,79 +18799,91 @@
       <c r="A345" s="62"/>
       <c r="B345" s="62"/>
     </row>
-    <row r="346" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A346" s="1" t="s">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" s="62"/>
+      <c r="B346" s="62"/>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" s="62"/>
+      <c r="B347" s="62"/>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="62"/>
+      <c r="B348" s="62"/>
+    </row>
+    <row r="349" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
         <v>1860</v>
       </c>
-      <c r="B346" s="2" t="s">
+      <c r="B349" s="2" t="s">
         <v>1861</v>
-      </c>
-    </row>
-    <row r="347" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A347" s="1" t="s">
-        <v>1862</v>
-      </c>
-      <c r="B347" s="2" t="s">
-        <v>1863</v>
-      </c>
-    </row>
-    <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A348" s="1" t="s">
-        <v>1865</v>
-      </c>
-      <c r="B348" s="2" t="s">
-        <v>1864</v>
-      </c>
-    </row>
-    <row r="349" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A349" s="1" t="s">
-        <v>1866</v>
-      </c>
-      <c r="B349" s="2" t="s">
-        <v>1867</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B350" s="2" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="B351" s="2" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B352" s="2" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
         <v>1868</v>
       </c>
-      <c r="B350" s="2" t="s">
+      <c r="B353" s="2" t="s">
         <v>1869</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A351" s="1" t="s">
+    <row r="354" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A354" s="1" t="s">
         <v>1870</v>
       </c>
-      <c r="B351" s="2" t="s">
+      <c r="B354" s="2" t="s">
         <v>1871</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A352" s="1" t="s">
+    <row r="355" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
         <v>1872</v>
       </c>
-      <c r="B352" s="2" t="s">
+      <c r="B355" s="2" t="s">
         <v>1873</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A353" s="1" t="s">
+    <row r="356" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
         <v>1874</v>
       </c>
-      <c r="B353" s="2" t="s">
+      <c r="B356" s="2" t="s">
         <v>1875</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A314:A316"/>
-    <mergeCell ref="A299:A300"/>
+    <mergeCell ref="A317:A319"/>
+    <mergeCell ref="A302:A303"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A109:A110"/>
     <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A291:B291"/>
-    <mergeCell ref="A295:A297"/>
+    <mergeCell ref="A294:B294"/>
+    <mergeCell ref="A298:A300"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -18878,10 +18905,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>894</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -19504,10 +19531,10 @@
       <c r="B79" s="23"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="65" t="s">
+      <c r="A80" s="66" t="s">
         <v>1214</v>
       </c>
-      <c r="B80" s="66"/>
+      <c r="B80" s="67"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -19715,10 +19742,10 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="65" t="s">
+      <c r="A107" s="66" t="s">
         <v>1220</v>
       </c>
-      <c r="B107" s="66"/>
+      <c r="B107" s="67"/>
     </row>
     <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="26" t="s">
@@ -19777,10 +19804,10 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="65" t="s">
+      <c r="A115" s="66" t="s">
         <v>1219</v>
       </c>
-      <c r="B115" s="66"/>
+      <c r="B115" s="67"/>
     </row>
     <row r="116" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
@@ -20063,10 +20090,10 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="65" t="s">
+      <c r="A152" s="66" t="s">
         <v>1185</v>
       </c>
-      <c r="B152" s="66"/>
+      <c r="B152" s="67"/>
     </row>
     <row r="153" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
@@ -20109,10 +20136,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>537</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -20411,10 +20438,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="68" t="s">
+      <c r="A39" s="69" t="s">
         <v>433</v>
       </c>
-      <c r="B39" s="68"/>
+      <c r="B39" s="69"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -20609,10 +20636,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="65" t="s">
+      <c r="A65" s="66" t="s">
         <v>498</v>
       </c>
-      <c r="B65" s="66"/>
+      <c r="B65" s="67"/>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
@@ -20775,10 +20802,10 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="65" t="s">
+      <c r="A87" s="66" t="s">
         <v>1236</v>
       </c>
-      <c r="B87" s="66"/>
+      <c r="B87" s="67"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
@@ -20815,10 +20842,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -21290,8 +21317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21301,10 +21328,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -21507,7 +21534,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="70" t="s">
         <v>1061</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -21515,13 +21542,13 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="69"/>
+      <c r="A28" s="70"/>
       <c r="B28" s="2" t="s">
         <v>1052</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="69" t="s">
+      <c r="A29" s="70" t="s">
         <v>1062</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -21529,13 +21556,13 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
+      <c r="A30" s="70"/>
       <c r="B30" s="2" t="s">
         <v>1054</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="67" t="s">
+      <c r="A31" s="68" t="s">
         <v>1063</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -21543,19 +21570,19 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="67"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="3" t="s">
         <v>1058</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="67"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="2" t="s">
         <v>1059</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A34" s="67"/>
+      <c r="A34" s="68"/>
       <c r="B34" s="2" t="s">
         <v>1060</v>
       </c>
@@ -21593,10 +21620,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="65" t="s">
+      <c r="A39" s="66" t="s">
         <v>979</v>
       </c>
-      <c r="B39" s="66"/>
+      <c r="B39" s="67"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -21647,10 +21674,10 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="65" t="s">
+      <c r="A47" s="66" t="s">
         <v>992</v>
       </c>
-      <c r="B47" s="66"/>
+      <c r="B47" s="67"/>
     </row>
     <row r="48" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="56" t="s">
@@ -21741,7 +21768,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A59" s="69" t="s">
+      <c r="A59" s="70" t="s">
         <v>1015</v>
       </c>
       <c r="B59" s="18" t="s">
@@ -21749,7 +21776,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A60" s="69"/>
+      <c r="A60" s="70"/>
       <c r="B60" s="18" t="s">
         <v>1017</v>
       </c>
@@ -21771,7 +21798,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="69" t="s">
+      <c r="A63" s="70" t="s">
         <v>1022</v>
       </c>
       <c r="B63" s="18" t="s">
@@ -21779,7 +21806,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A64" s="69"/>
+      <c r="A64" s="70"/>
       <c r="B64" s="18" t="s">
         <v>1024</v>
       </c>
@@ -21809,10 +21836,10 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="65" t="s">
+      <c r="A69" s="66" t="s">
         <v>1031</v>
       </c>
-      <c r="B69" s="66"/>
+      <c r="B69" s="67"/>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -21910,10 +21937,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>1218</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -22024,10 +22051,10 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="66" t="s">
         <v>1672</v>
       </c>
-      <c r="B16" s="66"/>
+      <c r="B16" s="67"/>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -22158,7 +22185,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="70" t="s">
         <v>1741</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -22166,7 +22193,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
+      <c r="A34" s="70"/>
       <c r="B34" s="2" t="s">
         <v>1744</v>
       </c>
@@ -22213,10 +22240,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>1454</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
@@ -22715,10 +22742,10 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="65" t="s">
+      <c r="A64" s="66" t="s">
         <v>1455</v>
       </c>
-      <c r="B64" s="66"/>
+      <c r="B64" s="67"/>
     </row>
     <row r="65" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="44" t="s">
@@ -23142,8 +23169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23153,10 +23180,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>604</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="67"/>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -23350,10 +23377,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="66" t="s">
         <v>1255</v>
       </c>
-      <c r="B27" s="66"/>
+      <c r="B27" s="67"/>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -23628,10 +23655,10 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="65" t="s">
+      <c r="A62" s="66" t="s">
         <v>1546</v>
       </c>
-      <c r="B62" s="66"/>
+      <c r="B62" s="67"/>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -23674,7 +23701,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="69" t="s">
+      <c r="A68" s="70" t="s">
         <v>1558</v>
       </c>
       <c r="B68" s="40" t="s">
@@ -23682,7 +23709,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="69"/>
+      <c r="A69" s="70"/>
       <c r="B69" s="40" t="s">
         <v>1560</v>
       </c>

</xml_diff>

<commit_message>
updated Core Java -> Garbage collection
updated Core Java -> Garbage collection
</commit_message>
<xml_diff>
--- a/Definitions.xlsx
+++ b/Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="2035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="2086">
   <si>
     <t>JDK</t>
   </si>
@@ -14669,6 +14669,194 @@
   </si>
   <si>
     <t>In general parent class loader will be asked to load the class first but where as in the case of WAR - class loader of specific WAR will try to load the class with in the same WAR, if class not found in the WAR then it will be delegated to EAR class loader and EAR deligates to Container class loader and container deligates to system class loaded and system class loader deligates to Bootstrap class loader. Only difference is WAR will check and deligate where as EAR first deligates and checks</t>
+  </si>
+  <si>
+    <t>http://commons.apache.org/proper/commons-bcel/</t>
+  </si>
+  <si>
+    <t>BCEL - Byte Code Engineering Library</t>
+  </si>
+  <si>
+    <t>Some classloaders</t>
+  </si>
+  <si>
+    <t>sun.misc.Launcher$AppClassLoader
+sun.misc.Launcher$ExtClassLoader
+java.net.URLClassLoader
+java.security.SecurityClassLoader
+java.rmi.server.RMIClassLoader
+sun.applet.AppletClassLoader</t>
+  </si>
+  <si>
+    <t>Design Patterns</t>
+  </si>
+  <si>
+    <t>Effective Java</t>
+  </si>
+  <si>
+    <t>RESTful web service</t>
+  </si>
+  <si>
+    <t>Refer JavaPrep/ClassLoading for more material</t>
+  </si>
+  <si>
+    <t>Garbage Collection Topics</t>
+  </si>
+  <si>
+    <t>Ways to make an object eligible for garbage collection
+1. Nullifying reference varable
+2. re assigning reference varable
+3. object created inside method
+4. Island of Isolation</t>
+  </si>
+  <si>
+    <t>Finalization</t>
+  </si>
+  <si>
+    <t>Brief intro to garbage collection</t>
+  </si>
+  <si>
+    <t>In Java, programmer is responsible only for creation of objects and he is not responsible for destruction of useless objects. SUN people provided one assistant which is always running in the background for distruction of useless objects. Just because of this assistant, the chance of failing java program with memory problems is very very less. This assistant is nothing but Garbage Collector</t>
+  </si>
+  <si>
+    <t>Main objective of garbage collector is to destroy objects</t>
+  </si>
+  <si>
+    <t>Garbage collector is best example for Daemon Thread as it is always running in the background.</t>
+  </si>
+  <si>
+    <t>Ways for requesting JVM to run GC
+1. Using System class --&gt; System.gc();
+2. Using Runtime class --&gt; Runtime.gc();</t>
+  </si>
+  <si>
+    <t>Objects which we are not using
+Useless objects</t>
+  </si>
+  <si>
+    <t>Process of garbage collector collecting garbage is called garbage collection</t>
+  </si>
+  <si>
+    <t>1. Garbage collector is responsible for collecting garbage
+2. Which is responsible for destroying useless objects</t>
+  </si>
+  <si>
+    <t>What is the grabage</t>
+  </si>
+  <si>
+    <t>what is Garbage collector</t>
+  </si>
+  <si>
+    <t>what is Garbage collection</t>
+  </si>
+  <si>
+    <t>Java is robust. What this means?</t>
+  </si>
+  <si>
+    <t>Chances for Java program to fail is very very less</t>
+  </si>
+  <si>
+    <t>One example to say Java is robust?</t>
+  </si>
+  <si>
+    <t>One example is garbage collector. Because of GC chances for java program to fail due to OutOfMemoryError is very very less</t>
+  </si>
+  <si>
+    <t>Note on making an object eligible for garbage collection</t>
+  </si>
+  <si>
+    <t>Even though programmer is not responsible to destroy useless objects but it is highly recommended to make an object eligible for GC if no longer required. An object said to be eligible GC if it doesn't contain any reference.</t>
+  </si>
+  <si>
+    <t>Ways to make an object eligible for garbage collection</t>
+  </si>
+  <si>
+    <t>1. Nullifying the reference variable
+2. re assigning reference variable
+3. object created inside method
+4. Islant of Isolation</t>
+  </si>
+  <si>
+    <t>Nullifying reference variable</t>
+  </si>
+  <si>
+    <t>If an object is no longer required, then assign null value to it's reference variables. Then object is automatically eligible for garbage collection</t>
+  </si>
+  <si>
+    <t>Example for nullifying reference variable</t>
+  </si>
+  <si>
+    <t>Re assigning reference variable</t>
+  </si>
+  <si>
+    <t>Objects created inside method</t>
+  </si>
+  <si>
+    <t>Objects created inside method are by default eligible for garbage collection once method completes (because reference variables are local variables of that method and once method completes all local variables will be destroyed)</t>
+  </si>
+  <si>
+    <t>Objects created inside method - Example</t>
+  </si>
+  <si>
+    <t>Objects created inside method - Example 2</t>
+  </si>
+  <si>
+    <t>Island of Isolation</t>
+  </si>
+  <si>
+    <t>Note on Island of Isolation</t>
+  </si>
+  <si>
+    <t>Even though object having reference variable still sometimes it may be eligible for garbage collection (if all references are internal references)</t>
+  </si>
+  <si>
+    <t>Ways for requesting JVM to run grabage collector</t>
+  </si>
+  <si>
+    <t>Once we made an object eligible for GC, it may not be destroyed immediately by the garbage collector. Whenever JVM runs the garbage collector then only objects will be destroyed. But when exactly JVM runs GC, we can't expect it. It depends on JVM and varies JVM to JVM</t>
+  </si>
+  <si>
+    <t>Instead of waiting until JVM runs GC, we can request JVM to run garbage collector. But there is no guarantee whether JVM accepts our request or not. But most of times JVM accepts our request</t>
+  </si>
+  <si>
+    <t>1. java.lang.System.gc();
+2. using java.lang.Runtime class</t>
+  </si>
+  <si>
+    <t>System.gc()</t>
+  </si>
+  <si>
+    <t>java.lang.System class contains static method gc() for the purpose of garbage collection</t>
+  </si>
+  <si>
+    <t>java.lang.Runtime class</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. A java application can communicate with JVM by using Runtime object
+2. Runtime class is singlton class
+3. We can create Runtime class by using getRuntime() method.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Runtime runtime = Runtime.getRuntime();</t>
+    </r>
+  </si>
+  <si>
+    <t>Once we create Runtime object, we need to call these methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. freeMemory() : returns number of bytes of free memory present in the heap
+2. totalMemory() : returns total number of bytes of heap (i.e Heap size)
+3. gc() : </t>
   </si>
 </sst>
 </file>
@@ -14859,7 +15047,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -15074,6 +15262,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -15095,6 +15289,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -15114,6 +15314,253 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>374</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5191125</xdr:colOff>
+      <xdr:row>386</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4105275" y="194033775"/>
+          <a:ext cx="5124450" cy="2419350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>387</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4743450</xdr:colOff>
+      <xdr:row>399</xdr:row>
+      <xdr:rowOff>88158</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4095751" y="196519800"/>
+          <a:ext cx="4686299" cy="2345583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95252</xdr:colOff>
+      <xdr:row>401</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6724650</xdr:colOff>
+      <xdr:row>411</xdr:row>
+      <xdr:rowOff>174635</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4133852" y="199367775"/>
+          <a:ext cx="6629398" cy="2060585"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>412</xdr:row>
+      <xdr:rowOff>41167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6029324</xdr:colOff>
+      <xdr:row>426</xdr:row>
+      <xdr:rowOff>107194</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095750" y="201485392"/>
+          <a:ext cx="5972174" cy="2733027"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>427</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7553325</xdr:colOff>
+      <xdr:row>438</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4124325" y="204311250"/>
+          <a:ext cx="7467600" cy="2200275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15403,10 +15850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:XFD98"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15593,15 +16040,15 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>261</v>
+      <c r="A27" s="19" t="s">
+        <v>262</v>
       </c>
       <c r="B27" s="72"/>
       <c r="C27" s="72"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>262</v>
+        <v>2010</v>
       </c>
       <c r="B28" s="72"/>
       <c r="C28" s="72"/>
@@ -15610,530 +16057,568 @@
       <c r="A29" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
+      <c r="B29" s="74"/>
+      <c r="C29" s="74"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>2010</v>
-      </c>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
+        <v>261</v>
+      </c>
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>2011</v>
-      </c>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
+        <v>2039</v>
+      </c>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>892</v>
-      </c>
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
+        <v>2040</v>
+      </c>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B33" s="27"/>
+        <v>2041</v>
+      </c>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>531</v>
-      </c>
+        <v>2011</v>
+      </c>
+      <c r="B34" s="72"/>
+      <c r="C34" s="72"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>267</v>
-      </c>
+        <v>1810</v>
+      </c>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>1907</v>
-      </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
+        <v>1721</v>
+      </c>
+      <c r="B36" s="72"/>
+      <c r="C36" s="72"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>1906</v>
-      </c>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
+        <v>2036</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="74"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>1802</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>1803</v>
-      </c>
-      <c r="C38" s="49"/>
+        <v>1234</v>
+      </c>
+      <c r="B38" s="27"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>1801</v>
-      </c>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
+        <v>531</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>892</v>
-      </c>
-      <c r="C40" s="27"/>
+        <v>267</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>1806</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>1807</v>
-      </c>
-      <c r="C41" s="49"/>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>1907</v>
+      </c>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>1804</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>1805</v>
-      </c>
-      <c r="C42" s="49"/>
-    </row>
-    <row r="43" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>1906</v>
+      </c>
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>260</v>
-      </c>
+        <v>1802</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C43" s="49"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>1801</v>
+      </c>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>892</v>
+      </c>
+      <c r="C45" s="27"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1806</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C46" s="49"/>
+    </row>
+    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>669</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1804</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C47" s="49"/>
+    </row>
+    <row r="48" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>1317</v>
+        <v>259</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>1248</v>
-      </c>
-      <c r="C49" s="41"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="B50" s="33" t="s">
-        <v>1246</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>616</v>
+        <v>669</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>1228</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>894</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>459</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>1180</v>
-      </c>
+        <v>1247</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C54" s="41"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>530</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
+      </c>
+      <c r="B55" s="33" t="s">
+        <v>1246</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>268</v>
+        <v>616</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>885</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>884</v>
+        <v>894</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>269</v>
+        <v>459</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>1180</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>270</v>
+        <v>530</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>233</v>
+        <v>282</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>273</v>
+        <v>885</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>884</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>1995</v>
-      </c>
-      <c r="B65" s="71"/>
-      <c r="C65" s="71"/>
+        <v>270</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>1720</v>
+        <v>233</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>373</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>289</v>
-      </c>
+        <v>1995</v>
+      </c>
+      <c r="B70" s="71"/>
+      <c r="C70" s="71"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>291</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>293</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>297</v>
+        <v>286</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>685</v>
+        <v>290</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>713</v>
+        <v>292</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>714</v>
+        <v>293</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>873</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>1799</v>
+        <v>294</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>874</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>875</v>
+        <v>296</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>876</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>877</v>
+        <v>315</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>878</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>881</v>
+        <v>713</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>880</v>
+        <v>714</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
-        <v>882</v>
+        <v>873</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>883</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>1548</v>
+        <v>874</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>1549</v>
+        <v>875</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>1576</v>
+        <v>876</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>877</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>1668</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>878</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>1686</v>
+        <v>881</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>1681</v>
+        <v>882</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>883</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
-        <v>1682</v>
+        <v>1548</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>1549</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>1683</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
-        <v>1684</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
-        <v>1719</v>
+        <v>1685</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>1686</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
-        <v>1721</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>1810</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
-        <v>1811</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>1812</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>1819</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>1820</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>1997</v>
-      </c>
-      <c r="B97" s="4"/>
-      <c r="C97" s="71"/>
+        <v>1719</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
+        <v>1997</v>
+      </c>
+      <c r="B102" s="4"/>
+      <c r="C102" s="71"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="s">
         <v>1998</v>
       </c>
-      <c r="B98" s="4"/>
-      <c r="C98" s="71"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="73" t="s">
+      <c r="B103" s="4"/>
+      <c r="C103" s="71"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="75" t="s">
         <v>1814</v>
       </c>
-      <c r="B99" s="74"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
+      <c r="B104" s="76"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="8" t="s">
         <v>1815</v>
       </c>
-      <c r="B100" s="50" t="s">
+      <c r="B105" s="50" t="s">
         <v>1816</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="8" t="s">
         <v>1817</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
         <v>1818</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A104:B104"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B77" r:id="rId2"/>
-    <hyperlink ref="B79" r:id="rId3"/>
-    <hyperlink ref="B80" r:id="rId4"/>
-    <hyperlink ref="B81" r:id="rId5"/>
-    <hyperlink ref="B82" r:id="rId6"/>
-    <hyperlink ref="B83" r:id="rId7"/>
-    <hyperlink ref="B58" r:id="rId8"/>
-    <hyperlink ref="B69" r:id="rId9"/>
-    <hyperlink ref="B54" r:id="rId10"/>
-    <hyperlink ref="B47" r:id="rId11"/>
+    <hyperlink ref="B82" r:id="rId2"/>
+    <hyperlink ref="B84" r:id="rId3"/>
+    <hyperlink ref="B85" r:id="rId4"/>
+    <hyperlink ref="B86" r:id="rId5"/>
+    <hyperlink ref="B87" r:id="rId6"/>
+    <hyperlink ref="B88" r:id="rId7"/>
+    <hyperlink ref="B63" r:id="rId8"/>
+    <hyperlink ref="B74" r:id="rId9"/>
+    <hyperlink ref="B59" r:id="rId10"/>
+    <hyperlink ref="B52" r:id="rId11"/>
     <hyperlink ref="B17" r:id="rId12"/>
-    <hyperlink ref="B49" r:id="rId13"/>
-    <hyperlink ref="B84" r:id="rId14"/>
-    <hyperlink ref="B78" r:id="rId15"/>
-    <hyperlink ref="B72" r:id="rId16"/>
-    <hyperlink ref="B38" r:id="rId17"/>
-    <hyperlink ref="B42" r:id="rId18" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
-    <hyperlink ref="B41" r:id="rId19"/>
-    <hyperlink ref="B95" r:id="rId20"/>
-    <hyperlink ref="B96" r:id="rId21"/>
+    <hyperlink ref="B54" r:id="rId13"/>
+    <hyperlink ref="B89" r:id="rId14"/>
+    <hyperlink ref="B83" r:id="rId15"/>
+    <hyperlink ref="B77" r:id="rId16"/>
+    <hyperlink ref="B43" r:id="rId17"/>
+    <hyperlink ref="B47" r:id="rId18" display="http://howtodoinjava.com/2014/04/13/java-8-tutorial-streams-by-examples/"/>
+    <hyperlink ref="B46" r:id="rId19"/>
+    <hyperlink ref="B100" r:id="rId20"/>
+    <hyperlink ref="B101" r:id="rId21"/>
+    <hyperlink ref="B37" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId22"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -16152,10 +16637,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>1770</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
@@ -16318,10 +16803,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>693</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
@@ -16369,10 +16854,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="75" t="s">
         <v>1821</v>
       </c>
-      <c r="B11" s="74"/>
+      <c r="B11" s="76"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
@@ -16463,10 +16948,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="73" t="s">
+      <c r="A29" s="75" t="s">
         <v>1842</v>
       </c>
-      <c r="B29" s="74"/>
+      <c r="B29" s="76"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
@@ -16494,10 +16979,10 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="73" t="s">
+      <c r="A36" s="75" t="s">
         <v>261</v>
       </c>
-      <c r="B36" s="74"/>
+      <c r="B36" s="76"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="51" t="s">
@@ -16535,13 +17020,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>1978</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="80" t="s">
         <v>1979</v>
       </c>
       <c r="B2" s="65" t="s">
@@ -16549,7 +17034,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A3" s="79"/>
+      <c r="A3" s="81"/>
       <c r="B3" s="65" t="s">
         <v>1980</v>
       </c>
@@ -16566,10 +17051,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B355"/>
+  <dimension ref="A1:B446"/>
   <sheetViews>
-    <sheetView topLeftCell="A343" workbookViewId="0">
-      <selection activeCell="B356" sqref="B356"/>
+    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
+      <selection activeCell="B446" sqref="B446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16579,10 +17064,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -16609,7 +17094,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="77" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -16617,7 +17102,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="75"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="2" t="s">
         <v>235</v>
       </c>
@@ -17439,7 +17924,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A109" s="75" t="s">
+      <c r="A109" s="77" t="s">
         <v>1993</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -17447,7 +17932,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="75"/>
+      <c r="A110" s="77"/>
       <c r="B110" s="2" t="s">
         <v>1762</v>
       </c>
@@ -17461,7 +17946,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A112" s="75" t="s">
+      <c r="A112" s="77" t="s">
         <v>1764</v>
       </c>
       <c r="B112" s="2" t="s">
@@ -17469,7 +17954,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A113" s="75"/>
+      <c r="A113" s="77"/>
       <c r="B113" s="2" t="s">
         <v>1767</v>
       </c>
@@ -18902,10 +19387,10 @@
       <c r="A293" s="64"/>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="73" t="s">
+      <c r="A294" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B294" s="74"/>
+      <c r="B294" s="76"/>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="53" t="s">
@@ -18932,7 +19417,7 @@
       </c>
     </row>
     <row r="298" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A298" s="75" t="s">
+      <c r="A298" s="77" t="s">
         <v>1873</v>
       </c>
       <c r="B298" s="53" t="s">
@@ -18940,13 +19425,13 @@
       </c>
     </row>
     <row r="299" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A299" s="75"/>
+      <c r="A299" s="77"/>
       <c r="B299" s="53" t="s">
         <v>1866</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A300" s="75"/>
+      <c r="A300" s="77"/>
       <c r="B300" s="53" t="s">
         <v>1867</v>
       </c>
@@ -18960,7 +19445,7 @@
       </c>
     </row>
     <row r="302" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A302" s="75" t="s">
+      <c r="A302" s="77" t="s">
         <v>1871</v>
       </c>
       <c r="B302" s="53" t="s">
@@ -18968,7 +19453,7 @@
       </c>
     </row>
     <row r="303" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A303" s="75"/>
+      <c r="A303" s="77"/>
       <c r="B303" s="53" t="s">
         <v>1921</v>
       </c>
@@ -19078,7 +19563,7 @@
       </c>
     </row>
     <row r="317" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A317" s="75" t="s">
+      <c r="A317" s="77" t="s">
         <v>1898</v>
       </c>
       <c r="B317" s="55" t="s">
@@ -19086,13 +19571,13 @@
       </c>
     </row>
     <row r="318" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A318" s="75"/>
+      <c r="A318" s="77"/>
       <c r="B318" s="55" t="s">
         <v>1900</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A319" s="75"/>
+      <c r="A319" s="77"/>
       <c r="B319" s="55" t="s">
         <v>1901</v>
       </c>
@@ -19250,10 +19735,10 @@
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="73" t="s">
+      <c r="A340" s="75" t="s">
         <v>1996</v>
       </c>
-      <c r="B340" s="74"/>
+      <c r="B340" s="76"/>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
@@ -19346,7 +19831,7 @@
       </c>
     </row>
     <row r="353" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A353" s="75" t="s">
+      <c r="A353" s="77" t="s">
         <v>2032</v>
       </c>
       <c r="B353" s="2" t="s">
@@ -19354,19 +19839,492 @@
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A354" s="75"/>
+      <c r="A354" s="77"/>
       <c r="B354" s="2" t="s">
         <v>2033</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A355" s="75"/>
+      <c r="A355" s="77"/>
       <c r="B355" s="2" t="s">
         <v>2034</v>
       </c>
     </row>
+    <row r="356" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
+        <v>2037</v>
+      </c>
+      <c r="B356" s="2" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="79" t="s">
+        <v>2042</v>
+      </c>
+      <c r="B357" s="79"/>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="75" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B359" s="76"/>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="82" t="s">
+        <v>2043</v>
+      </c>
+      <c r="B360" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A361" s="77"/>
+      <c r="B361" s="2" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A362" s="77"/>
+      <c r="B362" s="2" t="s">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="77"/>
+      <c r="B363" s="2" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A364" s="77" t="s">
+        <v>2046</v>
+      </c>
+      <c r="B364" s="2" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="77"/>
+      <c r="B365" s="2" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="77"/>
+      <c r="B366" s="2" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A367" s="73" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B367" s="2" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A368" s="73" t="s">
+        <v>2055</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="1" t="s">
+        <v>2056</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="1" t="s">
+        <v>2057</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="1" t="s">
+        <v>2059</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A372" s="1" t="s">
+        <v>2061</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A373" s="1" t="s">
+        <v>2063</v>
+      </c>
+      <c r="B373" s="2" t="s">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A374" s="1" t="s">
+        <v>2065</v>
+      </c>
+      <c r="B374" s="2" t="s">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" s="77" t="s">
+        <v>2067</v>
+      </c>
+      <c r="B375" s="83"/>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" s="77"/>
+      <c r="B376" s="83"/>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" s="77"/>
+      <c r="B377" s="83"/>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" s="77"/>
+      <c r="B378" s="83"/>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" s="77"/>
+      <c r="B379" s="83"/>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" s="77"/>
+      <c r="B380" s="83"/>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" s="77"/>
+      <c r="B381" s="83"/>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" s="77"/>
+      <c r="B382" s="83"/>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" s="77"/>
+      <c r="B383" s="83"/>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" s="77"/>
+      <c r="B384" s="83"/>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" s="77"/>
+      <c r="B385" s="83"/>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" s="77"/>
+      <c r="B386" s="83"/>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" s="77"/>
+      <c r="B387" s="83"/>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" s="77" t="s">
+        <v>2068</v>
+      </c>
+      <c r="B388" s="83"/>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" s="77"/>
+      <c r="B389" s="83"/>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" s="77"/>
+      <c r="B390" s="83"/>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" s="77"/>
+      <c r="B391" s="83"/>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" s="77"/>
+      <c r="B392" s="83"/>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" s="77"/>
+      <c r="B393" s="83"/>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" s="77"/>
+      <c r="B394" s="83"/>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" s="77"/>
+      <c r="B395" s="83"/>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" s="77"/>
+      <c r="B396" s="83"/>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" s="77"/>
+      <c r="B397" s="83"/>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398" s="77"/>
+      <c r="B398" s="83"/>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399" s="77"/>
+      <c r="B399" s="83"/>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400" s="77"/>
+      <c r="B400" s="83"/>
+    </row>
+    <row r="401" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A401" s="1" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B401" s="2" t="s">
+        <v>2070</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" s="77" t="s">
+        <v>2071</v>
+      </c>
+      <c r="B402" s="83"/>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" s="77"/>
+      <c r="B403" s="83"/>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" s="77"/>
+      <c r="B404" s="83"/>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" s="77"/>
+      <c r="B405" s="83"/>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" s="77"/>
+      <c r="B406" s="83"/>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" s="77"/>
+      <c r="B407" s="83"/>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" s="77"/>
+      <c r="B408" s="83"/>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" s="77"/>
+      <c r="B409" s="83"/>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" s="77"/>
+      <c r="B410" s="83"/>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" s="77"/>
+      <c r="B411" s="83"/>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412" s="77"/>
+      <c r="B412" s="83"/>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413" s="77" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B413" s="83"/>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414" s="77"/>
+      <c r="B414" s="83"/>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415" s="77"/>
+      <c r="B415" s="83"/>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416" s="77"/>
+      <c r="B416" s="83"/>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417" s="77"/>
+      <c r="B417" s="83"/>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418" s="77"/>
+      <c r="B418" s="83"/>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419" s="77"/>
+      <c r="B419" s="83"/>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420" s="77"/>
+      <c r="B420" s="83"/>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421" s="77"/>
+      <c r="B421" s="83"/>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422" s="77"/>
+      <c r="B422" s="83"/>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423" s="77"/>
+      <c r="B423" s="83"/>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424" s="77"/>
+      <c r="B424" s="83"/>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425" s="77"/>
+      <c r="B425" s="83"/>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426" s="77"/>
+      <c r="B426" s="83"/>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427" s="77"/>
+      <c r="B427" s="83"/>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428" s="77" t="s">
+        <v>2073</v>
+      </c>
+      <c r="B428" s="83"/>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A429" s="77"/>
+      <c r="B429" s="83"/>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430" s="77"/>
+      <c r="B430" s="83"/>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" s="77"/>
+      <c r="B431" s="83"/>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" s="77"/>
+      <c r="B432" s="83"/>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" s="77"/>
+      <c r="B433" s="83"/>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" s="77"/>
+      <c r="B434" s="83"/>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" s="77"/>
+      <c r="B435" s="83"/>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" s="77"/>
+      <c r="B436" s="83"/>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" s="77"/>
+      <c r="B437" s="83"/>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" s="77"/>
+      <c r="B438" s="83"/>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" s="77"/>
+      <c r="B439" s="83"/>
+    </row>
+    <row r="440" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A440" s="1" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B440" s="2" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A441" s="77" t="s">
+        <v>2076</v>
+      </c>
+      <c r="B441" s="2" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A442" s="77"/>
+      <c r="B442" s="2" t="s">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A443" s="1" t="s">
+        <v>2076</v>
+      </c>
+      <c r="B443" s="2" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" s="1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B444" s="2" t="s">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A445" s="73" t="s">
+        <v>2082</v>
+      </c>
+      <c r="B445" s="2" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A446" s="1" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B446" s="2" t="s">
+        <v>2085</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="25">
+    <mergeCell ref="B413:B427"/>
+    <mergeCell ref="A413:A427"/>
+    <mergeCell ref="B428:B439"/>
+    <mergeCell ref="A428:A439"/>
+    <mergeCell ref="A441:A442"/>
+    <mergeCell ref="B388:B400"/>
+    <mergeCell ref="A388:A400"/>
+    <mergeCell ref="B402:B412"/>
+    <mergeCell ref="A402:A412"/>
+    <mergeCell ref="A357:B357"/>
+    <mergeCell ref="A359:B359"/>
+    <mergeCell ref="A360:A363"/>
+    <mergeCell ref="A364:A366"/>
+    <mergeCell ref="A375:A387"/>
+    <mergeCell ref="B375:B387"/>
     <mergeCell ref="A353:A355"/>
     <mergeCell ref="A340:B340"/>
     <mergeCell ref="A317:A319"/>
@@ -19380,6 +20338,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -19387,8 +20346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152:B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19398,10 +20357,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>891</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -20024,10 +20983,10 @@
       <c r="B79" s="23"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="73" t="s">
+      <c r="A80" s="75" t="s">
         <v>1209</v>
       </c>
-      <c r="B80" s="74"/>
+      <c r="B80" s="76"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -20235,10 +21194,10 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="73" t="s">
+      <c r="A107" s="75" t="s">
         <v>1215</v>
       </c>
-      <c r="B107" s="74"/>
+      <c r="B107" s="76"/>
     </row>
     <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="26" t="s">
@@ -20297,10 +21256,10 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="73" t="s">
+      <c r="A115" s="75" t="s">
         <v>1214</v>
       </c>
-      <c r="B115" s="74"/>
+      <c r="B115" s="76"/>
     </row>
     <row r="116" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
@@ -20583,10 +21542,10 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="73" t="s">
+      <c r="A152" s="75" t="s">
         <v>1181</v>
       </c>
-      <c r="B152" s="74"/>
+      <c r="B152" s="76"/>
     </row>
     <row r="153" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
@@ -20618,7 +21577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
@@ -20629,10 +21588,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>535</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -20931,10 +21890,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="76" t="s">
+      <c r="A39" s="78" t="s">
         <v>432</v>
       </c>
-      <c r="B39" s="76"/>
+      <c r="B39" s="78"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -21129,10 +22088,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="73" t="s">
+      <c r="A65" s="75" t="s">
         <v>496</v>
       </c>
-      <c r="B65" s="74"/>
+      <c r="B65" s="76"/>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
@@ -21295,10 +22254,10 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="73" t="s">
+      <c r="A87" s="75" t="s">
         <v>1230</v>
       </c>
-      <c r="B87" s="74"/>
+      <c r="B87" s="76"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
@@ -21335,10 +22294,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -21821,10 +22780,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -22027,7 +22986,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="79" t="s">
         <v>1058</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -22035,13 +22994,13 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="77"/>
+      <c r="A28" s="79"/>
       <c r="B28" s="2" t="s">
         <v>1049</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="79" t="s">
         <v>1059</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -22049,13 +23008,13 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="77"/>
+      <c r="A30" s="79"/>
       <c r="B30" s="2" t="s">
         <v>1051</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="77" t="s">
         <v>1060</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -22063,19 +23022,19 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="75"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="3" t="s">
         <v>1055</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="75"/>
+      <c r="A33" s="77"/>
       <c r="B33" s="2" t="s">
         <v>1056</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A34" s="75"/>
+      <c r="A34" s="77"/>
       <c r="B34" s="2" t="s">
         <v>1057</v>
       </c>
@@ -22113,10 +23072,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="73" t="s">
+      <c r="A39" s="75" t="s">
         <v>976</v>
       </c>
-      <c r="B39" s="74"/>
+      <c r="B39" s="76"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -22167,10 +23126,10 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="73" t="s">
+      <c r="A47" s="75" t="s">
         <v>989</v>
       </c>
-      <c r="B47" s="74"/>
+      <c r="B47" s="76"/>
     </row>
     <row r="48" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="56" t="s">
@@ -22261,7 +23220,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A59" s="77" t="s">
+      <c r="A59" s="79" t="s">
         <v>1012</v>
       </c>
       <c r="B59" s="18" t="s">
@@ -22269,7 +23228,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A60" s="77"/>
+      <c r="A60" s="79"/>
       <c r="B60" s="18" t="s">
         <v>1014</v>
       </c>
@@ -22291,7 +23250,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="77" t="s">
+      <c r="A63" s="79" t="s">
         <v>1019</v>
       </c>
       <c r="B63" s="18" t="s">
@@ -22299,7 +23258,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A64" s="77"/>
+      <c r="A64" s="79"/>
       <c r="B64" s="18" t="s">
         <v>1021</v>
       </c>
@@ -22329,10 +23288,10 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="73" t="s">
+      <c r="A69" s="75" t="s">
         <v>1028</v>
       </c>
-      <c r="B69" s="74"/>
+      <c r="B69" s="76"/>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -22430,10 +23389,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>1213</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -22544,10 +23503,10 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="75" t="s">
         <v>1663</v>
       </c>
-      <c r="B16" s="74"/>
+      <c r="B16" s="76"/>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -22678,7 +23637,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="79" t="s">
         <v>1732</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -22686,7 +23645,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
+      <c r="A34" s="79"/>
       <c r="B34" s="2" t="s">
         <v>1735</v>
       </c>
@@ -22733,10 +23692,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>1446</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
@@ -23235,10 +24194,10 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="73" t="s">
+      <c r="A64" s="75" t="s">
         <v>1447</v>
       </c>
-      <c r="B64" s="74"/>
+      <c r="B64" s="76"/>
     </row>
     <row r="65" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="44" t="s">
@@ -23662,8 +24621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23673,10 +24632,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>602</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -23870,10 +24829,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="75" t="s">
         <v>1249</v>
       </c>
-      <c r="B27" s="74"/>
+      <c r="B27" s="76"/>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -24148,10 +25107,10 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="73" t="s">
+      <c r="A62" s="75" t="s">
         <v>1538</v>
       </c>
-      <c r="B62" s="74"/>
+      <c r="B62" s="76"/>
     </row>
     <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -24194,7 +25153,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="77" t="s">
+      <c r="A68" s="79" t="s">
         <v>1550</v>
       </c>
       <c r="B68" s="40" t="s">
@@ -24202,7 +25161,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="77"/>
+      <c r="A69" s="79"/>
       <c r="B69" s="40" t="s">
         <v>1552</v>
       </c>
@@ -24304,10 +25263,10 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="73" t="s">
+      <c r="A84" s="75" t="s">
         <v>873</v>
       </c>
-      <c r="B84" s="74"/>
+      <c r="B84" s="76"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="66" t="s">

</xml_diff>

<commit_message>
updated core java - garbage collection
updated core java - garbage collection
</commit_message>
<xml_diff>
--- a/Definitions.xlsx
+++ b/Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="10515" windowHeight="4680" tabRatio="764" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2136" uniqueCount="2085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="2094">
   <si>
     <t>JDK</t>
   </si>
@@ -14854,6 +14854,34 @@
   </si>
   <si>
     <t>Example of using Runtime object for garbage collection</t>
+  </si>
+  <si>
+    <t>System.gc() vs Runtime.getRuntime.gc()</t>
+  </si>
+  <si>
+    <t>Just before destroying an object garbage collector calls finalize() method to perform cleanup activities. Once finalize() completes automatically GC destroys that objet.
+java.lang.Object.protected void finalize() throws Throwable { }</t>
+  </si>
+  <si>
+    <t>We can override finalize() method in our class to perform clean up activities</t>
+  </si>
+  <si>
+    <t>Example 1</t>
+  </si>
+  <si>
+    <t>Can we call finalize() method explicitely? Yes</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>What happens if exception occurs while executing finalize method</t>
+  </si>
+  <si>
+    <t>In programmer calls finalize method explicitely and while executing finaliza() if any exception occurs and which is uncaught then program will be terminated abnormally by raising that exception</t>
+  </si>
+  <si>
+    <t>If garbage collector calls finalize() method and while executing finalize() method, if any exception occurs and which is uncaught then JVM ignores that exception and rest of the program will be executed normally</t>
   </si>
 </sst>
 </file>
@@ -15274,11 +15302,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -15604,6 +15632,226 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>458</xdr:row>
+      <xdr:rowOff>35694</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6554485</xdr:colOff>
+      <xdr:row>472</xdr:row>
+      <xdr:rowOff>133903</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4171950" y="211805019"/>
+          <a:ext cx="6421135" cy="2765209"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>475</xdr:row>
+      <xdr:rowOff>24826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5792532</xdr:colOff>
+      <xdr:row>487</xdr:row>
+      <xdr:rowOff>181554</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4210050" y="215413651"/>
+          <a:ext cx="5621082" cy="2442728"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>103726</xdr:colOff>
+      <xdr:row>488</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5411507</xdr:colOff>
+      <xdr:row>500</xdr:row>
+      <xdr:rowOff>95818</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4142326" y="217941525"/>
+          <a:ext cx="5307781" cy="2305618"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>501</xdr:row>
+      <xdr:rowOff>61284</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6602225</xdr:colOff>
+      <xdr:row>509</xdr:row>
+      <xdr:rowOff>86059</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4143375" y="220403109"/>
+          <a:ext cx="6497450" cy="1548775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>512</xdr:row>
+      <xdr:rowOff>57131</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4897234</xdr:colOff>
+      <xdr:row>523</xdr:row>
+      <xdr:rowOff>133974</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4124325" y="222875456"/>
+          <a:ext cx="4811509" cy="2172343"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -15896,7 +16144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -17070,10 +17318,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B458"/>
+  <dimension ref="A1:B524"/>
   <sheetViews>
-    <sheetView topLeftCell="A444" workbookViewId="0">
-      <selection activeCell="A447" sqref="A447:A458"/>
+    <sheetView tabSelected="1" topLeftCell="A511" workbookViewId="0">
+      <selection activeCell="A513" sqref="A513:A524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17113,7 +17361,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="78" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -17121,7 +17369,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
+      <c r="A6" s="78"/>
       <c r="B6" s="2" t="s">
         <v>235</v>
       </c>
@@ -17943,7 +18191,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A109" s="79" t="s">
+      <c r="A109" s="78" t="s">
         <v>1992</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -17951,7 +18199,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="79"/>
+      <c r="A110" s="78"/>
       <c r="B110" s="2" t="s">
         <v>1761</v>
       </c>
@@ -17965,7 +18213,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A112" s="79" t="s">
+      <c r="A112" s="78" t="s">
         <v>1763</v>
       </c>
       <c r="B112" s="2" t="s">
@@ -17973,7 +18221,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A113" s="79"/>
+      <c r="A113" s="78"/>
       <c r="B113" s="2" t="s">
         <v>1766</v>
       </c>
@@ -19436,7 +19684,7 @@
       </c>
     </row>
     <row r="298" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A298" s="79" t="s">
+      <c r="A298" s="78" t="s">
         <v>1872</v>
       </c>
       <c r="B298" s="53" t="s">
@@ -19444,13 +19692,13 @@
       </c>
     </row>
     <row r="299" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A299" s="79"/>
+      <c r="A299" s="78"/>
       <c r="B299" s="53" t="s">
         <v>1865</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A300" s="79"/>
+      <c r="A300" s="78"/>
       <c r="B300" s="53" t="s">
         <v>1866</v>
       </c>
@@ -19464,7 +19712,7 @@
       </c>
     </row>
     <row r="302" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A302" s="79" t="s">
+      <c r="A302" s="78" t="s">
         <v>1870</v>
       </c>
       <c r="B302" s="53" t="s">
@@ -19472,7 +19720,7 @@
       </c>
     </row>
     <row r="303" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A303" s="79"/>
+      <c r="A303" s="78"/>
       <c r="B303" s="53" t="s">
         <v>1920</v>
       </c>
@@ -19582,7 +19830,7 @@
       </c>
     </row>
     <row r="317" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A317" s="79" t="s">
+      <c r="A317" s="78" t="s">
         <v>1897</v>
       </c>
       <c r="B317" s="55" t="s">
@@ -19590,13 +19838,13 @@
       </c>
     </row>
     <row r="318" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A318" s="79"/>
+      <c r="A318" s="78"/>
       <c r="B318" s="55" t="s">
         <v>1899</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A319" s="79"/>
+      <c r="A319" s="78"/>
       <c r="B319" s="55" t="s">
         <v>1900</v>
       </c>
@@ -19850,7 +20098,7 @@
       </c>
     </row>
     <row r="353" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A353" s="79" t="s">
+      <c r="A353" s="78" t="s">
         <v>2030</v>
       </c>
       <c r="B353" s="2" t="s">
@@ -19858,13 +20106,13 @@
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A354" s="79"/>
+      <c r="A354" s="78"/>
       <c r="B354" s="2" t="s">
         <v>2031</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A355" s="79"/>
+      <c r="A355" s="78"/>
       <c r="B355" s="2" t="s">
         <v>2032</v>
       </c>
@@ -19898,25 +20146,25 @@
       </c>
     </row>
     <row r="361" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A361" s="79"/>
+      <c r="A361" s="78"/>
       <c r="B361" s="2" t="s">
         <v>2042</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A362" s="79"/>
+      <c r="A362" s="78"/>
       <c r="B362" s="2" t="s">
         <v>2048</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A363" s="79"/>
+      <c r="A363" s="78"/>
       <c r="B363" s="2" t="s">
         <v>2043</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A364" s="79" t="s">
+      <c r="A364" s="78" t="s">
         <v>2044</v>
       </c>
       <c r="B364" s="2" t="s">
@@ -19924,13 +20172,13 @@
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A365" s="79"/>
+      <c r="A365" s="78"/>
       <c r="B365" s="2" t="s">
         <v>2046</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A366" s="79"/>
+      <c r="A366" s="78"/>
       <c r="B366" s="2" t="s">
         <v>2047</v>
       </c>
@@ -20000,112 +20248,112 @@
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A375" s="79" t="s">
+      <c r="A375" s="78" t="s">
         <v>2065</v>
       </c>
-      <c r="B375" s="78"/>
+      <c r="B375" s="79"/>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A376" s="79"/>
-      <c r="B376" s="78"/>
+      <c r="A376" s="78"/>
+      <c r="B376" s="79"/>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A377" s="79"/>
-      <c r="B377" s="78"/>
+      <c r="A377" s="78"/>
+      <c r="B377" s="79"/>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A378" s="79"/>
-      <c r="B378" s="78"/>
+      <c r="A378" s="78"/>
+      <c r="B378" s="79"/>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A379" s="79"/>
-      <c r="B379" s="78"/>
+      <c r="A379" s="78"/>
+      <c r="B379" s="79"/>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A380" s="79"/>
-      <c r="B380" s="78"/>
+      <c r="A380" s="78"/>
+      <c r="B380" s="79"/>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A381" s="79"/>
-      <c r="B381" s="78"/>
+      <c r="A381" s="78"/>
+      <c r="B381" s="79"/>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A382" s="79"/>
-      <c r="B382" s="78"/>
+      <c r="A382" s="78"/>
+      <c r="B382" s="79"/>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A383" s="79"/>
-      <c r="B383" s="78"/>
+      <c r="A383" s="78"/>
+      <c r="B383" s="79"/>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A384" s="79"/>
-      <c r="B384" s="78"/>
+      <c r="A384" s="78"/>
+      <c r="B384" s="79"/>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" s="79"/>
-      <c r="B385" s="78"/>
+      <c r="A385" s="78"/>
+      <c r="B385" s="79"/>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" s="79"/>
-      <c r="B386" s="78"/>
+      <c r="A386" s="78"/>
+      <c r="B386" s="79"/>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" s="79"/>
-      <c r="B387" s="78"/>
+      <c r="A387" s="78"/>
+      <c r="B387" s="79"/>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" s="79" t="s">
+      <c r="A388" s="78" t="s">
         <v>2066</v>
       </c>
-      <c r="B388" s="78"/>
+      <c r="B388" s="79"/>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A389" s="79"/>
-      <c r="B389" s="78"/>
+      <c r="A389" s="78"/>
+      <c r="B389" s="79"/>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A390" s="79"/>
-      <c r="B390" s="78"/>
+      <c r="A390" s="78"/>
+      <c r="B390" s="79"/>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A391" s="79"/>
-      <c r="B391" s="78"/>
+      <c r="A391" s="78"/>
+      <c r="B391" s="79"/>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A392" s="79"/>
-      <c r="B392" s="78"/>
+      <c r="A392" s="78"/>
+      <c r="B392" s="79"/>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A393" s="79"/>
-      <c r="B393" s="78"/>
+      <c r="A393" s="78"/>
+      <c r="B393" s="79"/>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A394" s="79"/>
-      <c r="B394" s="78"/>
+      <c r="A394" s="78"/>
+      <c r="B394" s="79"/>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A395" s="79"/>
-      <c r="B395" s="78"/>
+      <c r="A395" s="78"/>
+      <c r="B395" s="79"/>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A396" s="79"/>
-      <c r="B396" s="78"/>
+      <c r="A396" s="78"/>
+      <c r="B396" s="79"/>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A397" s="79"/>
-      <c r="B397" s="78"/>
+      <c r="A397" s="78"/>
+      <c r="B397" s="79"/>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" s="79"/>
-      <c r="B398" s="78"/>
+      <c r="A398" s="78"/>
+      <c r="B398" s="79"/>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A399" s="79"/>
-      <c r="B399" s="78"/>
+      <c r="A399" s="78"/>
+      <c r="B399" s="79"/>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A400" s="79"/>
-      <c r="B400" s="78"/>
+      <c r="A400" s="78"/>
+      <c r="B400" s="79"/>
     </row>
     <row r="401" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
@@ -20116,162 +20364,162 @@
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A402" s="79" t="s">
+      <c r="A402" s="78" t="s">
         <v>2069</v>
       </c>
-      <c r="B402" s="78"/>
+      <c r="B402" s="79"/>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A403" s="79"/>
-      <c r="B403" s="78"/>
+      <c r="A403" s="78"/>
+      <c r="B403" s="79"/>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A404" s="79"/>
-      <c r="B404" s="78"/>
+      <c r="A404" s="78"/>
+      <c r="B404" s="79"/>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A405" s="79"/>
-      <c r="B405" s="78"/>
+      <c r="A405" s="78"/>
+      <c r="B405" s="79"/>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A406" s="79"/>
-      <c r="B406" s="78"/>
+      <c r="A406" s="78"/>
+      <c r="B406" s="79"/>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A407" s="79"/>
-      <c r="B407" s="78"/>
+      <c r="A407" s="78"/>
+      <c r="B407" s="79"/>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A408" s="79"/>
-      <c r="B408" s="78"/>
+      <c r="A408" s="78"/>
+      <c r="B408" s="79"/>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" s="79"/>
-      <c r="B409" s="78"/>
+      <c r="A409" s="78"/>
+      <c r="B409" s="79"/>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A410" s="79"/>
-      <c r="B410" s="78"/>
+      <c r="A410" s="78"/>
+      <c r="B410" s="79"/>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A411" s="79"/>
-      <c r="B411" s="78"/>
+      <c r="A411" s="78"/>
+      <c r="B411" s="79"/>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A412" s="79"/>
-      <c r="B412" s="78"/>
+      <c r="A412" s="78"/>
+      <c r="B412" s="79"/>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A413" s="79" t="s">
+      <c r="A413" s="78" t="s">
         <v>2070</v>
       </c>
-      <c r="B413" s="78"/>
+      <c r="B413" s="79"/>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A414" s="79"/>
-      <c r="B414" s="78"/>
+      <c r="A414" s="78"/>
+      <c r="B414" s="79"/>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A415" s="79"/>
-      <c r="B415" s="78"/>
+      <c r="A415" s="78"/>
+      <c r="B415" s="79"/>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A416" s="79"/>
-      <c r="B416" s="78"/>
+      <c r="A416" s="78"/>
+      <c r="B416" s="79"/>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A417" s="79"/>
-      <c r="B417" s="78"/>
+      <c r="A417" s="78"/>
+      <c r="B417" s="79"/>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A418" s="79"/>
-      <c r="B418" s="78"/>
+      <c r="A418" s="78"/>
+      <c r="B418" s="79"/>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A419" s="79"/>
-      <c r="B419" s="78"/>
+      <c r="A419" s="78"/>
+      <c r="B419" s="79"/>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A420" s="79"/>
-      <c r="B420" s="78"/>
+      <c r="A420" s="78"/>
+      <c r="B420" s="79"/>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A421" s="79"/>
-      <c r="B421" s="78"/>
+      <c r="A421" s="78"/>
+      <c r="B421" s="79"/>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A422" s="79"/>
-      <c r="B422" s="78"/>
+      <c r="A422" s="78"/>
+      <c r="B422" s="79"/>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A423" s="79"/>
-      <c r="B423" s="78"/>
+      <c r="A423" s="78"/>
+      <c r="B423" s="79"/>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A424" s="79"/>
-      <c r="B424" s="78"/>
+      <c r="A424" s="78"/>
+      <c r="B424" s="79"/>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A425" s="79"/>
-      <c r="B425" s="78"/>
+      <c r="A425" s="78"/>
+      <c r="B425" s="79"/>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A426" s="79"/>
-      <c r="B426" s="78"/>
+      <c r="A426" s="78"/>
+      <c r="B426" s="79"/>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A427" s="79"/>
-      <c r="B427" s="78"/>
+      <c r="A427" s="78"/>
+      <c r="B427" s="79"/>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A428" s="79" t="s">
+      <c r="A428" s="78" t="s">
         <v>2071</v>
       </c>
-      <c r="B428" s="78"/>
+      <c r="B428" s="79"/>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A429" s="79"/>
-      <c r="B429" s="78"/>
+      <c r="A429" s="78"/>
+      <c r="B429" s="79"/>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A430" s="79"/>
-      <c r="B430" s="78"/>
+      <c r="A430" s="78"/>
+      <c r="B430" s="79"/>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A431" s="79"/>
-      <c r="B431" s="78"/>
+      <c r="A431" s="78"/>
+      <c r="B431" s="79"/>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A432" s="79"/>
-      <c r="B432" s="78"/>
+      <c r="A432" s="78"/>
+      <c r="B432" s="79"/>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A433" s="79"/>
-      <c r="B433" s="78"/>
+      <c r="A433" s="78"/>
+      <c r="B433" s="79"/>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A434" s="79"/>
-      <c r="B434" s="78"/>
+      <c r="A434" s="78"/>
+      <c r="B434" s="79"/>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A435" s="79"/>
-      <c r="B435" s="78"/>
+      <c r="A435" s="78"/>
+      <c r="B435" s="79"/>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A436" s="79"/>
-      <c r="B436" s="78"/>
+      <c r="A436" s="78"/>
+      <c r="B436" s="79"/>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A437" s="79"/>
-      <c r="B437" s="78"/>
+      <c r="A437" s="78"/>
+      <c r="B437" s="79"/>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A438" s="79"/>
-      <c r="B438" s="78"/>
+      <c r="A438" s="78"/>
+      <c r="B438" s="79"/>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A439" s="79"/>
-      <c r="B439" s="78"/>
+      <c r="A439" s="78"/>
+      <c r="B439" s="79"/>
     </row>
     <row r="440" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
@@ -20282,7 +20530,7 @@
       </c>
     </row>
     <row r="441" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A441" s="79" t="s">
+      <c r="A441" s="78" t="s">
         <v>2074</v>
       </c>
       <c r="B441" s="2" t="s">
@@ -20290,7 +20538,7 @@
       </c>
     </row>
     <row r="442" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A442" s="79"/>
+      <c r="A442" s="78"/>
       <c r="B442" s="2" t="s">
         <v>2076</v>
       </c>
@@ -20328,57 +20576,372 @@
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A447" s="79" t="s">
+      <c r="A447" s="78" t="s">
         <v>2084</v>
       </c>
-      <c r="B447" s="78"/>
+      <c r="B447" s="79"/>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A448" s="79"/>
-      <c r="B448" s="78"/>
+      <c r="A448" s="78"/>
+      <c r="B448" s="79"/>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A449" s="79"/>
-      <c r="B449" s="78"/>
+      <c r="A449" s="78"/>
+      <c r="B449" s="79"/>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A450" s="79"/>
-      <c r="B450" s="78"/>
+      <c r="A450" s="78"/>
+      <c r="B450" s="79"/>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A451" s="79"/>
-      <c r="B451" s="78"/>
+      <c r="A451" s="78"/>
+      <c r="B451" s="79"/>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A452" s="79"/>
-      <c r="B452" s="78"/>
+      <c r="A452" s="78"/>
+      <c r="B452" s="79"/>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A453" s="79"/>
-      <c r="B453" s="78"/>
+      <c r="A453" s="78"/>
+      <c r="B453" s="79"/>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A454" s="79"/>
-      <c r="B454" s="78"/>
+      <c r="A454" s="78"/>
+      <c r="B454" s="79"/>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A455" s="79"/>
-      <c r="B455" s="78"/>
+      <c r="A455" s="78"/>
+      <c r="B455" s="79"/>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A456" s="79"/>
-      <c r="B456" s="78"/>
+      <c r="A456" s="78"/>
+      <c r="B456" s="79"/>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A457" s="79"/>
-      <c r="B457" s="78"/>
+      <c r="A457" s="78"/>
+      <c r="B457" s="79"/>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A458" s="79"/>
-      <c r="B458" s="78"/>
+      <c r="A458" s="78"/>
+      <c r="B458" s="79"/>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459" s="78" t="s">
+        <v>2085</v>
+      </c>
+      <c r="B459" s="79"/>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460" s="78"/>
+      <c r="B460" s="79"/>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A461" s="78"/>
+      <c r="B461" s="79"/>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A462" s="78"/>
+      <c r="B462" s="79"/>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A463" s="78"/>
+      <c r="B463" s="79"/>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A464" s="78"/>
+      <c r="B464" s="79"/>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A465" s="78"/>
+      <c r="B465" s="79"/>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A466" s="78"/>
+      <c r="B466" s="79"/>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467" s="78"/>
+      <c r="B467" s="79"/>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" s="78"/>
+      <c r="B468" s="79"/>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469" s="78"/>
+      <c r="B469" s="79"/>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470" s="78"/>
+      <c r="B470" s="79"/>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471" s="78"/>
+      <c r="B471" s="79"/>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472" s="78"/>
+      <c r="B472" s="79"/>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" s="78"/>
+      <c r="B473" s="79"/>
+    </row>
+    <row r="474" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A474" s="78" t="s">
+        <v>2043</v>
+      </c>
+      <c r="B474" s="2" t="s">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" s="78"/>
+      <c r="B475" s="2" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476" s="78" t="s">
+        <v>2088</v>
+      </c>
+      <c r="B476" s="79"/>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A477" s="78"/>
+      <c r="B477" s="79"/>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A478" s="78"/>
+      <c r="B478" s="79"/>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A479" s="78"/>
+      <c r="B479" s="79"/>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A480" s="78"/>
+      <c r="B480" s="79"/>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A481" s="78"/>
+      <c r="B481" s="79"/>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A482" s="78"/>
+      <c r="B482" s="79"/>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483" s="78"/>
+      <c r="B483" s="79"/>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A484" s="78"/>
+      <c r="B484" s="79"/>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485" s="78"/>
+      <c r="B485" s="79"/>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A486" s="78"/>
+      <c r="B486" s="79"/>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A487" s="78"/>
+      <c r="B487" s="79"/>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A488" s="78"/>
+      <c r="B488" s="79"/>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A489" s="78" t="s">
+        <v>2089</v>
+      </c>
+      <c r="B489" s="79"/>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A490" s="78"/>
+      <c r="B490" s="79"/>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A491" s="78"/>
+      <c r="B491" s="79"/>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492" s="78"/>
+      <c r="B492" s="79"/>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A493" s="78"/>
+      <c r="B493" s="79"/>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A494" s="78"/>
+      <c r="B494" s="79"/>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A495" s="78"/>
+      <c r="B495" s="79"/>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A496" s="78"/>
+      <c r="B496" s="79"/>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497" s="78"/>
+      <c r="B497" s="79"/>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498" s="78"/>
+      <c r="B498" s="79"/>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A499" s="78"/>
+      <c r="B499" s="79"/>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A500" s="78"/>
+      <c r="B500" s="79"/>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A501" s="78"/>
+      <c r="B501" s="79"/>
+    </row>
+    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A502" s="78" t="s">
+        <v>2090</v>
+      </c>
+      <c r="B502" s="79"/>
+    </row>
+    <row r="503" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A503" s="78"/>
+      <c r="B503" s="79"/>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A504" s="78"/>
+      <c r="B504" s="79"/>
+    </row>
+    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A505" s="78"/>
+      <c r="B505" s="79"/>
+    </row>
+    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A506" s="78"/>
+      <c r="B506" s="79"/>
+    </row>
+    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A507" s="78"/>
+      <c r="B507" s="79"/>
+    </row>
+    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A508" s="78"/>
+      <c r="B508" s="79"/>
+    </row>
+    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A509" s="78"/>
+      <c r="B509" s="79"/>
+    </row>
+    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A510" s="78"/>
+      <c r="B510" s="79"/>
+    </row>
+    <row r="511" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A511" s="78" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B511" s="2" t="s">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A512" s="78"/>
+      <c r="B512" s="2" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A513" s="78" t="s">
+        <v>2090</v>
+      </c>
+      <c r="B513" s="79"/>
+    </row>
+    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A514" s="78"/>
+      <c r="B514" s="79"/>
+    </row>
+    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A515" s="78"/>
+      <c r="B515" s="79"/>
+    </row>
+    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A516" s="78"/>
+      <c r="B516" s="79"/>
+    </row>
+    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A517" s="78"/>
+      <c r="B517" s="79"/>
+    </row>
+    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A518" s="78"/>
+      <c r="B518" s="79"/>
+    </row>
+    <row r="519" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A519" s="78"/>
+      <c r="B519" s="79"/>
+    </row>
+    <row r="520" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A520" s="78"/>
+      <c r="B520" s="79"/>
+    </row>
+    <row r="521" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A521" s="78"/>
+      <c r="B521" s="79"/>
+    </row>
+    <row r="522" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A522" s="78"/>
+      <c r="B522" s="79"/>
+    </row>
+    <row r="523" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A523" s="78"/>
+      <c r="B523" s="79"/>
+    </row>
+    <row r="524" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A524" s="78"/>
+      <c r="B524" s="79"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="39">
+    <mergeCell ref="B513:B524"/>
+    <mergeCell ref="A513:A524"/>
+    <mergeCell ref="B489:B501"/>
+    <mergeCell ref="A489:A501"/>
+    <mergeCell ref="B502:B510"/>
+    <mergeCell ref="A502:A510"/>
+    <mergeCell ref="A511:A512"/>
+    <mergeCell ref="B459:B473"/>
+    <mergeCell ref="A459:A473"/>
+    <mergeCell ref="A474:A475"/>
+    <mergeCell ref="B476:B488"/>
+    <mergeCell ref="A476:A488"/>
+    <mergeCell ref="B447:B458"/>
+    <mergeCell ref="A447:A458"/>
+    <mergeCell ref="B413:B427"/>
+    <mergeCell ref="A413:A427"/>
+    <mergeCell ref="B428:B439"/>
+    <mergeCell ref="A428:A439"/>
+    <mergeCell ref="A441:A442"/>
+    <mergeCell ref="B388:B400"/>
+    <mergeCell ref="A388:A400"/>
+    <mergeCell ref="B402:B412"/>
+    <mergeCell ref="A402:A412"/>
+    <mergeCell ref="A357:B357"/>
+    <mergeCell ref="A359:B359"/>
+    <mergeCell ref="A360:A363"/>
+    <mergeCell ref="A364:A366"/>
+    <mergeCell ref="A375:A387"/>
+    <mergeCell ref="B375:B387"/>
     <mergeCell ref="A353:A355"/>
     <mergeCell ref="A340:B340"/>
     <mergeCell ref="A317:A319"/>
@@ -20389,23 +20952,6 @@
     <mergeCell ref="A294:B294"/>
     <mergeCell ref="A298:A300"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B388:B400"/>
-    <mergeCell ref="A388:A400"/>
-    <mergeCell ref="B402:B412"/>
-    <mergeCell ref="A402:A412"/>
-    <mergeCell ref="A357:B357"/>
-    <mergeCell ref="A359:B359"/>
-    <mergeCell ref="A360:A363"/>
-    <mergeCell ref="A364:A366"/>
-    <mergeCell ref="A375:A387"/>
-    <mergeCell ref="B375:B387"/>
-    <mergeCell ref="B447:B458"/>
-    <mergeCell ref="A447:A458"/>
-    <mergeCell ref="B413:B427"/>
-    <mergeCell ref="A413:A427"/>
-    <mergeCell ref="B428:B439"/>
-    <mergeCell ref="A428:A439"/>
-    <mergeCell ref="A441:A442"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -23085,7 +23631,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="78" t="s">
         <v>1059</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -23093,19 +23639,19 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="79"/>
+      <c r="A32" s="78"/>
       <c r="B32" s="3" t="s">
         <v>1054</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="79"/>
+      <c r="A33" s="78"/>
       <c r="B33" s="2" t="s">
         <v>1055</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A34" s="79"/>
+      <c r="A34" s="78"/>
       <c r="B34" s="2" t="s">
         <v>1056</v>
       </c>

</xml_diff>